<commit_message>
Koch & al sub-national GDP data
</commit_message>
<xml_diff>
--- a/data/raw_control_variables/Austrian_industrial_statistics_1854.xlsx
+++ b/data/raw_control_variables/Austrian_industrial_statistics_1854.xlsx
@@ -1,37 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miro8\OneDrive - Universiteit Utrecht\Documents\Github\layout_parse\data\raw_control_variables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://solisservices-my.sharepoint.com/personal/g_domini_uu_nl/Documents/Documents/Github/layout_parse/data/raw_control_variables/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="77" documentId="11_EA4A92EB7895B9A7F3CC3FE6396E1A3CB926333B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F543C94-EF64-42ED-B33F-A30BF678B177}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="p133" sheetId="2" r:id="rId1"/>
     <sheet name="p159" sheetId="1" r:id="rId2"/>
     <sheet name="notes" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Giacomo Domini</author>
   </authors>
   <commentList>
-    <comment ref="G6" authorId="0" shapeId="0">
+    <comment ref="G6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -55,7 +67,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G16" authorId="0" shapeId="0">
+    <comment ref="G16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -79,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A46" authorId="0" shapeId="0">
+    <comment ref="A46" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -103,7 +115,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A47" authorId="0" shapeId="0">
+    <comment ref="A47" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -127,7 +139,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A67" authorId="0" shapeId="0">
+    <comment ref="A67" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -156,12 +168,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Giacomo Domini</author>
   </authors>
   <commentList>
-    <comment ref="I7" authorId="0" shapeId="0">
+    <comment ref="I7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -185,7 +197,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H8" authorId="0" shapeId="0">
+    <comment ref="H8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -209,7 +221,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I8" authorId="0" shapeId="0">
+    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -233,7 +245,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I11" authorId="0" shapeId="0">
+    <comment ref="I11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -257,7 +269,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C77" authorId="0" shapeId="0">
+    <comment ref="C77" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -286,7 +298,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="259">
   <si>
     <t>i . Maschinen - Flachsgarn - Spinnereien im Jahre 1854.</t>
   </si>
@@ -1039,12 +1051,36 @@
   </si>
   <si>
     <t>Total-Summe</t>
+  </si>
+  <si>
+    <t>RCA Lombardy (industry only)</t>
+  </si>
+  <si>
+    <t>RCA Veneto (industry only)</t>
+  </si>
+  <si>
+    <t>Share in total Lombardy</t>
+  </si>
+  <si>
+    <t>Share in total Veneto</t>
+  </si>
+  <si>
+    <t>Share in total Austria</t>
+  </si>
+  <si>
+    <t>Share in total Austria (industry)</t>
+  </si>
+  <si>
+    <t>Share in total Lombardy (industry)</t>
+  </si>
+  <si>
+    <t>Share in total Veneto (industry)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1158,9 +1194,27 @@
     <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1460,20 +1514,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M77"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:U77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A75" sqref="A75:XFD75"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L56" sqref="L56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>183</v>
       </c>
@@ -1490,19 +1545,37 @@
         <v>42</v>
       </c>
       <c r="I1" t="s">
+        <v>255</v>
+      </c>
+      <c r="J1" t="s">
+        <v>253</v>
+      </c>
+      <c r="K1" t="s">
+        <v>254</v>
+      </c>
+      <c r="M1" t="s">
+        <v>256</v>
+      </c>
+      <c r="N1" t="s">
+        <v>257</v>
+      </c>
+      <c r="O1" t="s">
+        <v>258</v>
+      </c>
+      <c r="Q1" t="s">
         <v>194</v>
       </c>
-      <c r="J1" t="s">
+      <c r="R1" t="s">
         <v>195</v>
       </c>
-      <c r="L1" t="s">
-        <v>194</v>
-      </c>
-      <c r="M1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>251</v>
+      </c>
+      <c r="U1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>184</v>
       </c>
@@ -1528,23 +1601,47 @@
         <v>1262</v>
       </c>
       <c r="I2" s="9">
-        <f>(F2/F$74)/($E2/E$74)</f>
-        <v>1.2651183363858645</v>
+        <f>100*E2/E$74</f>
+        <v>1.5675500636301571</v>
       </c>
       <c r="J2" s="9">
-        <f>(G2/G$74)/($E2/F$74)</f>
-        <v>0.301097398269082</v>
-      </c>
-      <c r="L2" s="9">
-        <f>IF($C2&lt;&gt;"", (F2/F$75)/($E2/E$75), "")</f>
+        <f t="shared" ref="J2:J48" si="0">100*F2/F$74</f>
+        <v>1.9831363287013402</v>
+      </c>
+      <c r="K2" s="9">
+        <f t="shared" ref="K2:K48" si="1">100*G2/G$74</f>
+        <v>1.2837597273790753</v>
+      </c>
+      <c r="M2" s="9">
+        <f>100*E2/E$75</f>
+        <v>1.9871151271753682</v>
+      </c>
+      <c r="N2" s="9">
+        <f t="shared" ref="N2:N48" si="2">100*F2/F$75</f>
+        <v>2.7178509372164901</v>
+      </c>
+      <c r="O2" s="9">
+        <f t="shared" ref="O2:O48" si="3">100*G2/G$75</f>
+        <v>1.9469900336326329</v>
+      </c>
+      <c r="Q2" s="9">
+        <f>J2/$I2</f>
+        <v>1.2651183363858642</v>
+      </c>
+      <c r="R2" s="9">
+        <f t="shared" ref="R2:R48" si="4">K2/$I2</f>
+        <v>0.81895931566365687</v>
+      </c>
+      <c r="T2" s="9">
+        <f>IF($C2&lt;&gt;"", N2/$M2, "")</f>
         <v>1.3677370274362732</v>
       </c>
-      <c r="M2" s="9">
-        <f>IF($C2&lt;&gt;"", (G2/G$75)/($E2/F$75), "")</f>
-        <v>0.33320684962429215</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="U2" s="9">
+        <f t="shared" ref="U2:U48" si="5">IF($C2&lt;&gt;"", O2/$M2, "")</f>
+        <v>0.97980736345167274</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>184</v>
       </c>
@@ -1567,23 +1664,47 @@
         <v>8303</v>
       </c>
       <c r="I3" s="9">
-        <f>(F3/F$74)/($E3/E$74)</f>
-        <v>5.3545713536291872</v>
+        <f t="shared" ref="I3:I66" si="6">100*E3/E$74</f>
+        <v>1.6778973378462274</v>
       </c>
       <c r="J3" s="9">
-        <f>(G3/G$74)/($E3/F$74)</f>
-        <v>1.8507114884320581</v>
-      </c>
-      <c r="L3" s="9">
-        <f>IF($C3&lt;&gt;"", (F3/F$75)/($E3/E$75), "")</f>
-        <v>5.7889015563003223</v>
+        <f t="shared" si="0"/>
+        <v>8.9844210195620828</v>
+      </c>
+      <c r="K3" s="9">
+        <f t="shared" si="1"/>
+        <v>8.4461624535883217</v>
       </c>
       <c r="M3" s="9">
-        <f>IF($C3&lt;&gt;"", (G3/G$75)/($E3/F$75), "")</f>
-        <v>2.048073972638019</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <f t="shared" ref="M3:M48" si="7">100*E3/E$75</f>
+        <v>2.1269975736278446</v>
+      </c>
+      <c r="N3" s="9">
+        <f t="shared" si="2"/>
+        <v>12.312979564221241</v>
+      </c>
+      <c r="O3" s="9">
+        <f t="shared" si="3"/>
+        <v>12.809713351229597</v>
+      </c>
+      <c r="Q3" s="9">
+        <f t="shared" ref="Q3:Q48" si="8">J3/$I3</f>
+        <v>5.3545713536291863</v>
+      </c>
+      <c r="R3" s="9">
+        <f t="shared" si="4"/>
+        <v>5.0337778498593568</v>
+      </c>
+      <c r="T3" s="9">
+        <f t="shared" ref="T3:T48" si="9">IF($C3&lt;&gt;"", N3/$M3, "")</f>
+        <v>5.7889015563003232</v>
+      </c>
+      <c r="U3" s="9">
+        <f t="shared" si="5"/>
+        <v>6.0224390991575625</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>184</v>
       </c>
@@ -1606,23 +1727,47 @@
         <v>531</v>
       </c>
       <c r="I4" s="9">
-        <f>(F4/F$74)/($E4/E$74)</f>
+        <f t="shared" si="6"/>
+        <v>0.62887633473794069</v>
+      </c>
+      <c r="J4" s="9">
+        <f t="shared" si="0"/>
+        <v>0.16269010900237302</v>
+      </c>
+      <c r="K4" s="9">
+        <f t="shared" si="1"/>
+        <v>0.54015563806520528</v>
+      </c>
+      <c r="M4" s="9">
+        <f t="shared" si="7"/>
+        <v>0.79719921352074963</v>
+      </c>
+      <c r="N4" s="9">
+        <f t="shared" si="2"/>
+        <v>0.22296372610828349</v>
+      </c>
+      <c r="O4" s="9">
+        <f t="shared" si="3"/>
+        <v>0.81921688419883365</v>
+      </c>
+      <c r="Q4" s="9">
+        <f t="shared" si="8"/>
         <v>0.25869968388962783</v>
       </c>
-      <c r="J4" s="9">
-        <f>(G4/G$74)/($E4/F$74)</f>
-        <v>0.31578997360458189</v>
-      </c>
-      <c r="L4" s="9">
-        <f>IF($C4&lt;&gt;"", (F4/F$75)/($E4/E$75), "")</f>
-        <v>0.27968382598320279</v>
-      </c>
-      <c r="M4" s="9">
-        <f>IF($C4&lt;&gt;"", (G4/G$75)/($E4/F$75), "")</f>
-        <v>0.3494662619226156</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="R4" s="9">
+        <f t="shared" si="4"/>
+        <v>0.85892187100710948</v>
+      </c>
+      <c r="T4" s="9">
+        <f t="shared" si="9"/>
+        <v>0.27968382598320285</v>
+      </c>
+      <c r="U4" s="9">
+        <f t="shared" si="5"/>
+        <v>1.0276187812339217</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>184</v>
       </c>
@@ -1641,23 +1786,38 @@
         <v>411</v>
       </c>
       <c r="I5" s="9">
-        <f>(F5/F$74)/($E5/E$74)</f>
+        <f t="shared" si="6"/>
+        <v>0.2442077993865929</v>
+      </c>
+      <c r="J5" s="9">
+        <f t="shared" si="0"/>
+        <v>0.35567423830173966</v>
+      </c>
+      <c r="K5" s="9">
+        <f t="shared" si="1"/>
+        <v>0.4180865673160063</v>
+      </c>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="Q5" s="9">
+        <f t="shared" si="8"/>
         <v>1.456440945764758</v>
       </c>
-      <c r="J5" s="9">
-        <f>(G5/G$74)/($E5/F$74)</f>
-        <v>0.6294356831400344</v>
-      </c>
-      <c r="L5" s="9" t="str">
-        <f>IF($C5&lt;&gt;"", (F5/F$75)/($E5/E$75), "")</f>
+      <c r="R5" s="9">
+        <f t="shared" si="4"/>
+        <v>1.7120115261108217</v>
+      </c>
+      <c r="T5" s="9" t="str">
+        <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="M5" s="9" t="str">
-        <f>IF($C5&lt;&gt;"", (G5/G$75)/($E5/F$75), "")</f>
+      <c r="U5" s="9" t="str">
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>186</v>
       </c>
@@ -1683,23 +1843,47 @@
         <v>772</v>
       </c>
       <c r="I6" s="9">
-        <f>(F6/F$74)/($E6/E$74)</f>
+        <f t="shared" si="6"/>
+        <v>0.2782401362943529</v>
+      </c>
+      <c r="J6" s="9">
+        <f t="shared" si="0"/>
+        <v>0.43197028942009391</v>
+      </c>
+      <c r="K6" s="9">
+        <f t="shared" si="1"/>
+        <v>0.78531102181984636</v>
+      </c>
+      <c r="M6" s="9">
+        <f t="shared" si="7"/>
+        <v>0.35271293507362783</v>
+      </c>
+      <c r="N6" s="9">
+        <f t="shared" si="2"/>
+        <v>0.5920071348392355</v>
+      </c>
+      <c r="O6" s="9">
+        <f t="shared" si="3"/>
+        <v>1.1910271838069673</v>
+      </c>
+      <c r="Q6" s="9">
+        <f t="shared" si="8"/>
         <v>1.5525089053403438</v>
       </c>
-      <c r="J6" s="9">
-        <f>(G6/G$74)/($E6/F$74)</f>
-        <v>1.0376875135096597</v>
-      </c>
-      <c r="L6" s="9">
-        <f>IF($C6&lt;&gt;"", (F6/F$75)/($E6/E$75), "")</f>
-        <v>1.6784389682665186</v>
-      </c>
-      <c r="M6" s="9">
-        <f>IF($C6&lt;&gt;"", (G6/G$75)/($E6/F$75), "")</f>
-        <v>1.1483479739735878</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="R6" s="9">
+        <f t="shared" si="4"/>
+        <v>2.8224217838545704</v>
+      </c>
+      <c r="T6" s="9">
+        <f t="shared" si="9"/>
+        <v>1.6784389682665188</v>
+      </c>
+      <c r="U6" s="9">
+        <f t="shared" si="5"/>
+        <v>3.3767607177727794</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>186</v>
       </c>
@@ -1722,23 +1906,47 @@
         <v>216</v>
       </c>
       <c r="I7" s="9">
-        <f>(F7/F$74)/($E7/E$74)</f>
-        <v>1.1958691136012258</v>
+        <f t="shared" si="6"/>
+        <v>0.65300835545435232</v>
       </c>
       <c r="J7" s="9">
-        <f>(G7/G$74)/($E7/F$74)</f>
-        <v>0.12370979318655249</v>
-      </c>
-      <c r="L7" s="9">
-        <f>IF($C7&lt;&gt;"", (F7/F$75)/($E7/E$75), "")</f>
-        <v>1.2928707296365665</v>
+        <f t="shared" si="0"/>
+        <v>0.7809125232113906</v>
+      </c>
+      <c r="K7" s="9">
+        <f t="shared" si="1"/>
+        <v>0.21972432734855807</v>
       </c>
       <c r="M7" s="9">
-        <f>IF($C7&lt;&gt;"", (G7/G$75)/($E7/F$75), "")</f>
-        <v>0.13690238006814628</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0.82779032797858099</v>
+      </c>
+      <c r="N7" s="9">
+        <f t="shared" si="2"/>
+        <v>1.0702258853197608</v>
+      </c>
+      <c r="O7" s="9">
+        <f t="shared" si="3"/>
+        <v>0.33324076645376283</v>
+      </c>
+      <c r="Q7" s="9">
+        <f t="shared" si="8"/>
+        <v>1.1958691136012261</v>
+      </c>
+      <c r="R7" s="9">
+        <f t="shared" si="4"/>
+        <v>0.33648011623936658</v>
+      </c>
+      <c r="T7" s="9">
+        <f t="shared" si="9"/>
+        <v>1.2928707296365667</v>
+      </c>
+      <c r="U7" s="9">
+        <f t="shared" si="5"/>
+        <v>0.40256663455771302</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>186</v>
       </c>
@@ -1761,23 +1969,47 @@
         <v>22085</v>
       </c>
       <c r="I8" s="9">
-        <f>(F8/F$74)/($E8/E$74)</f>
+        <f t="shared" si="6"/>
+        <v>27.430476060829193</v>
+      </c>
+      <c r="J8" s="9">
+        <f t="shared" si="0"/>
+        <v>15.70688852361531</v>
+      </c>
+      <c r="K8" s="9">
+        <f t="shared" si="1"/>
+        <v>22.465795229133818</v>
+      </c>
+      <c r="M8" s="9">
+        <f t="shared" si="7"/>
+        <v>34.772423025435074</v>
+      </c>
+      <c r="N8" s="9">
+        <f t="shared" si="2"/>
+        <v>21.525994495102488</v>
+      </c>
+      <c r="O8" s="9">
+        <f t="shared" si="3"/>
+        <v>34.072325588571076</v>
+      </c>
+      <c r="Q8" s="9">
+        <f t="shared" si="8"/>
         <v>0.57260721574004314</v>
       </c>
-      <c r="J8" s="9">
-        <f>(G8/G$74)/($E8/F$74)</f>
-        <v>0.30111551048023866</v>
-      </c>
-      <c r="L8" s="9">
-        <f>IF($C8&lt;&gt;"", (F8/F$75)/($E8/E$75), "")</f>
+      <c r="R8" s="9">
+        <f t="shared" si="4"/>
+        <v>0.81900857933760196</v>
+      </c>
+      <c r="T8" s="9">
+        <f t="shared" si="9"/>
         <v>0.61905362417099352</v>
       </c>
-      <c r="M8" s="9">
-        <f>IF($C8&lt;&gt;"", (G8/G$75)/($E8/F$75), "")</f>
-        <v>0.33322689334720029</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="U8" s="9">
+        <f t="shared" si="5"/>
+        <v>0.97986630277815567</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>186</v>
       </c>
@@ -1799,23 +2031,47 @@
         <v>90</v>
       </c>
       <c r="I9" s="9">
-        <f>(F9/F$74)/($E9/E$74)</f>
+        <f t="shared" si="6"/>
+        <v>3.3619823733120474E-2</v>
+      </c>
+      <c r="J9" s="9">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J9" s="9">
-        <f>(G9/G$74)/($E9/F$74)</f>
-        <v>1.0011891749197985</v>
-      </c>
-      <c r="L9" s="9">
-        <f>IF($C9&lt;&gt;"", (F9/F$75)/($E9/E$75), "")</f>
+      <c r="K9" s="9">
+        <f t="shared" si="1"/>
+        <v>9.1551803061899195E-2</v>
+      </c>
+      <c r="M9" s="9">
+        <f t="shared" si="7"/>
+        <v>4.2618390227576977E-2</v>
+      </c>
+      <c r="N9" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M9" s="9">
-        <f>IF($C9&lt;&gt;"", (G9/G$75)/($E9/F$75), "")</f>
-        <v>1.1079574010627586</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O9" s="9">
+        <f t="shared" si="3"/>
+        <v>0.13885031935573452</v>
+      </c>
+      <c r="Q9" s="9">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="R9" s="9">
+        <f t="shared" si="4"/>
+        <v>2.72314940698833</v>
+      </c>
+      <c r="T9" s="9">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U9" s="9">
+        <f t="shared" si="5"/>
+        <v>3.2579907081025552</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>186</v>
       </c>
@@ -1838,23 +2094,47 @@
         <v>80</v>
       </c>
       <c r="I10" s="9">
-        <f>(F10/F$74)/($E10/E$74)</f>
-        <v>1.531447715102227</v>
+        <f t="shared" si="6"/>
+        <v>7.0333496276037313E-2</v>
       </c>
       <c r="J10" s="9">
-        <f>(G10/G$74)/($E10/F$74)</f>
-        <v>0.42539937572349862</v>
-      </c>
-      <c r="L10" s="9">
-        <f>IF($C10&lt;&gt;"", (F10/F$75)/($E10/E$75), "")</f>
-        <v>1.6556694226026372</v>
+        <f t="shared" si="0"/>
+        <v>0.10771207216708835</v>
+      </c>
+      <c r="K10" s="9">
+        <f t="shared" si="1"/>
+        <v>8.1379380499465942E-2</v>
       </c>
       <c r="M10" s="9">
-        <f>IF($C10&lt;&gt;"", (G10/G$75)/($E10/F$75), "")</f>
-        <v>0.47076456532611183</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>8.9158718206157964E-2</v>
+      </c>
+      <c r="N10" s="9">
+        <f t="shared" si="2"/>
+        <v>0.1476173634923808</v>
+      </c>
+      <c r="O10" s="9">
+        <f t="shared" si="3"/>
+        <v>0.12342250609398624</v>
+      </c>
+      <c r="Q10" s="9">
+        <f t="shared" si="8"/>
+        <v>1.5314477151022272</v>
+      </c>
+      <c r="R10" s="9">
+        <f t="shared" si="4"/>
+        <v>1.1570501227477294</v>
+      </c>
+      <c r="T10" s="9">
+        <f t="shared" si="9"/>
+        <v>1.6556694226026374</v>
+      </c>
+      <c r="U10" s="9">
+        <f t="shared" si="5"/>
+        <v>1.3843010372648197</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>186</v>
       </c>
@@ -1873,23 +2153,38 @@
         <v>13654</v>
       </c>
       <c r="I11" s="9">
-        <f>(F11/F$74)/($E11/E$74)</f>
-        <v>0.56564441710160251</v>
+        <f t="shared" si="6"/>
+        <v>10.773812838647535</v>
       </c>
       <c r="J11" s="9">
-        <f>(G11/G$74)/($E11/F$74)</f>
-        <v>0.47397947950604707</v>
-      </c>
-      <c r="L11" s="9" t="str">
-        <f>IF($C11&lt;&gt;"", (F11/F$75)/($E11/E$75), "")</f>
+        <f t="shared" si="0"/>
+        <v>6.0941470830785454</v>
+      </c>
+      <c r="K11" s="9">
+        <f t="shared" si="1"/>
+        <v>13.889425766746351</v>
+      </c>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="Q11" s="9">
+        <f t="shared" si="8"/>
+        <v>0.5656444171016024</v>
+      </c>
+      <c r="R11" s="9">
+        <f t="shared" si="4"/>
+        <v>1.2891838734122587</v>
+      </c>
+      <c r="T11" s="9" t="str">
+        <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="M11" s="9" t="str">
-        <f>IF($C11&lt;&gt;"", (G11/G$75)/($E11/F$75), "")</f>
+      <c r="U11" s="9" t="str">
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>187</v>
       </c>
@@ -1912,23 +2207,47 @@
         <v>33</v>
       </c>
       <c r="I12" s="9">
-        <f>(F12/F$74)/($E12/E$74)</f>
-        <v>3.4447858464058706E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.76541819554362023</v>
       </c>
       <c r="J12" s="9">
-        <f>(G12/G$74)/($E12/F$74)</f>
-        <v>1.6124424599220324E-2</v>
-      </c>
-      <c r="L12" s="9">
-        <f>IF($C12&lt;&gt;"", (F12/F$75)/($E12/E$75), "")</f>
+        <f t="shared" si="0"/>
+        <v>2.6367017665901837E-2</v>
+      </c>
+      <c r="K12" s="9">
+        <f t="shared" si="1"/>
+        <v>3.3568994456029705E-2</v>
+      </c>
+      <c r="M12" s="9">
+        <f t="shared" si="7"/>
+        <v>0.97028739959839361</v>
+      </c>
+      <c r="N12" s="9">
+        <f t="shared" si="2"/>
+        <v>3.613550043823905E-2</v>
+      </c>
+      <c r="O12" s="9">
+        <f t="shared" si="3"/>
+        <v>5.0911783763769321E-2</v>
+      </c>
+      <c r="Q12" s="9">
+        <f t="shared" si="8"/>
+        <v>3.4447858464058699E-2</v>
+      </c>
+      <c r="R12" s="9">
+        <f t="shared" si="4"/>
+        <v>4.3857063565346938E-2</v>
+      </c>
+      <c r="T12" s="9">
+        <f t="shared" si="9"/>
         <v>3.724205885101229E-2</v>
       </c>
-      <c r="M12" s="9">
-        <f>IF($C12&lt;&gt;"", (G12/G$75)/($E12/F$75), "")</f>
-        <v>1.7843955987654057E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="U12" s="9">
+        <f t="shared" si="5"/>
+        <v>5.2470828524457745E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>187</v>
       </c>
@@ -1951,23 +2270,47 @@
         <v>4212</v>
       </c>
       <c r="I13" s="9">
-        <f>(F13/F$74)/($E13/E$74)</f>
-        <v>0.39558291589926731</v>
+        <f t="shared" si="6"/>
+        <v>10.429158081236219</v>
       </c>
       <c r="J13" s="9">
-        <f>(G13/G$74)/($E13/F$74)</f>
-        <v>0.15104563527328121</v>
-      </c>
-      <c r="L13" s="9">
-        <f>IF($C13&lt;&gt;"", (F13/F$75)/($E13/E$75), "")</f>
-        <v>0.42767019174055709</v>
+        <f t="shared" si="0"/>
+        <v>4.1255967641498321</v>
+      </c>
+      <c r="K13" s="9">
+        <f t="shared" si="1"/>
+        <v>4.2846243832968822</v>
       </c>
       <c r="M13" s="9">
-        <f>IF($C13&lt;&gt;"", (G13/G$75)/($E13/F$75), "")</f>
-        <v>0.16715335492182476</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>13.220590696117805</v>
+      </c>
+      <c r="N13" s="9">
+        <f t="shared" si="2"/>
+        <v>5.6540525579321264</v>
+      </c>
+      <c r="O13" s="9">
+        <f t="shared" si="3"/>
+        <v>6.4981949458483754</v>
+      </c>
+      <c r="Q13" s="9">
+        <f t="shared" si="8"/>
+        <v>0.39558291589926742</v>
+      </c>
+      <c r="R13" s="9">
+        <f t="shared" si="4"/>
+        <v>0.41083128186594758</v>
+      </c>
+      <c r="T13" s="9">
+        <f t="shared" si="9"/>
+        <v>0.42767019174055704</v>
+      </c>
+      <c r="U13" s="9">
+        <f t="shared" si="5"/>
+        <v>0.49152077204512162</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>187</v>
       </c>
@@ -1990,23 +2333,47 @@
         <v>336</v>
       </c>
       <c r="I14" s="9">
-        <f>(F14/F$74)/($E14/E$74)</f>
-        <v>0.23212014089003299</v>
+        <f t="shared" si="6"/>
+        <v>0.5051223823460862</v>
       </c>
       <c r="J14" s="9">
-        <f>(G14/G$74)/($E14/F$74)</f>
-        <v>0.24877786276488148</v>
-      </c>
-      <c r="L14" s="9">
-        <f>IF($C14&lt;&gt;"", (F14/F$75)/($E14/E$75), "")</f>
+        <f t="shared" si="0"/>
+        <v>0.11724907855688263</v>
+      </c>
+      <c r="K14" s="9">
+        <f t="shared" si="1"/>
+        <v>0.341793398097757</v>
+      </c>
+      <c r="M14" s="9">
+        <f t="shared" si="7"/>
+        <v>0.64032170348058903</v>
+      </c>
+      <c r="N14" s="9">
+        <f t="shared" si="2"/>
+        <v>0.16068765088493533</v>
+      </c>
+      <c r="O14" s="9">
+        <f t="shared" si="3"/>
+        <v>0.51837452559474217</v>
+      </c>
+      <c r="Q14" s="9">
+        <f t="shared" si="8"/>
+        <v>0.23212014089003297</v>
+      </c>
+      <c r="R14" s="9">
+        <f t="shared" si="4"/>
+        <v>0.67665462874614046</v>
+      </c>
+      <c r="T14" s="9">
+        <f t="shared" si="9"/>
         <v>0.25094831240529158</v>
       </c>
-      <c r="M14" s="9">
-        <f>IF($C14&lt;&gt;"", (G14/G$75)/($E14/F$75), "")</f>
-        <v>0.27530788503881481</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="U14" s="9">
+        <f t="shared" si="5"/>
+        <v>0.80955326483081858</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>187</v>
       </c>
@@ -2025,23 +2392,38 @@
         <v>327</v>
       </c>
       <c r="I15" s="9">
-        <f>(F15/F$74)/($E15/E$74)</f>
+        <f t="shared" si="6"/>
+        <v>0.37249939669948207</v>
+      </c>
+      <c r="J15" s="9">
+        <f t="shared" si="0"/>
+        <v>0.36408924393979342</v>
+      </c>
+      <c r="K15" s="9">
+        <f t="shared" si="1"/>
+        <v>0.33263821779156705</v>
+      </c>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="Q15" s="9">
+        <f t="shared" si="8"/>
         <v>0.97742237213212557</v>
       </c>
-      <c r="J15" s="9">
-        <f>(G15/G$74)/($E15/F$74)</f>
-        <v>0.32831539444075419</v>
-      </c>
-      <c r="L15" s="9" t="str">
-        <f>IF($C15&lt;&gt;"", (F15/F$75)/($E15/E$75), "")</f>
+      <c r="R15" s="9">
+        <f t="shared" si="4"/>
+        <v>0.89298995042380314</v>
+      </c>
+      <c r="T15" s="9" t="str">
+        <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="M15" s="9" t="str">
-        <f>IF($C15&lt;&gt;"", (G15/G$75)/($E15/F$75), "")</f>
+      <c r="U15" s="9" t="str">
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>188</v>
       </c>
@@ -2065,23 +2447,47 @@
         <v>269</v>
       </c>
       <c r="I16" s="9">
-        <f>(F16/F$74)/($E16/E$74)</f>
+        <f t="shared" si="6"/>
+        <v>5.7751844449532106E-3</v>
+      </c>
+      <c r="J16" s="9">
+        <f t="shared" si="0"/>
+        <v>1.7475161708358344</v>
+      </c>
+      <c r="K16" s="9">
+        <f t="shared" si="1"/>
+        <v>0.27363816692945425</v>
+      </c>
+      <c r="M16" s="9">
+        <f t="shared" si="7"/>
+        <v>7.3209504685408299E-3</v>
+      </c>
+      <c r="N16" s="9">
+        <f t="shared" si="2"/>
+        <v>2.3949379545769069</v>
+      </c>
+      <c r="O16" s="9">
+        <f t="shared" si="3"/>
+        <v>0.41500817674102874</v>
+      </c>
+      <c r="Q16" s="9">
+        <f t="shared" si="8"/>
         <v>302.59053844816077</v>
       </c>
-      <c r="J16" s="9">
-        <f>(G16/G$74)/($E16/F$74)</f>
-        <v>17.420294346312861</v>
-      </c>
-      <c r="L16" s="9">
-        <f>IF($C16&lt;&gt;"", (F16/F$75)/($E16/E$75), "")</f>
+      <c r="R16" s="9">
+        <f t="shared" si="4"/>
+        <v>47.381719066752893</v>
+      </c>
+      <c r="T16" s="9">
+        <f t="shared" si="9"/>
         <v>327.13483923546505</v>
       </c>
-      <c r="M16" s="9">
-        <f>IF($C16&lt;&gt;"", (G16/G$75)/($E16/F$75), "")</f>
-        <v>19.278019112856658</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="U16" s="9">
+        <f t="shared" si="5"/>
+        <v>56.687745467528863</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>188</v>
       </c>
@@ -2104,23 +2510,47 @@
         <v>4100</v>
       </c>
       <c r="I17" s="9">
-        <f>(F17/F$74)/($E17/E$74)</f>
+        <f t="shared" si="6"/>
+        <v>6.7883168018678592</v>
+      </c>
+      <c r="J17" s="9">
+        <f t="shared" si="0"/>
+        <v>3.266144188316606</v>
+      </c>
+      <c r="K17" s="9">
+        <f t="shared" si="1"/>
+        <v>4.1706932505976297</v>
+      </c>
+      <c r="M17" s="9">
+        <f t="shared" si="7"/>
+        <v>8.6052543507362778</v>
+      </c>
+      <c r="N17" s="9">
+        <f t="shared" si="2"/>
+        <v>4.4761890117325054</v>
+      </c>
+      <c r="O17" s="9">
+        <f t="shared" si="3"/>
+        <v>6.3254034373167949</v>
+      </c>
+      <c r="Q17" s="9">
+        <f t="shared" si="8"/>
         <v>0.48114198020603582</v>
       </c>
-      <c r="J17" s="9">
-        <f>(G17/G$74)/($E17/F$74)</f>
-        <v>0.22588678415130628</v>
-      </c>
-      <c r="L17" s="9">
-        <f>IF($C17&lt;&gt;"", (F17/F$75)/($E17/E$75), "")</f>
+      <c r="R17" s="9">
+        <f t="shared" si="4"/>
+        <v>0.6143928417498179</v>
+      </c>
+      <c r="T17" s="9">
+        <f t="shared" si="9"/>
         <v>0.52016928603040258</v>
       </c>
-      <c r="M17" s="9">
-        <f>IF($C17&lt;&gt;"", (G17/G$75)/($E17/F$75), "")</f>
-        <v>0.24997566950596928</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="U17" s="9">
+        <f t="shared" si="5"/>
+        <v>0.73506292545270135</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>188</v>
       </c>
@@ -2142,23 +2572,47 @@
         <v>836</v>
       </c>
       <c r="I18" s="9">
-        <f>(F18/F$74)/($E18/E$74)</f>
+        <f t="shared" si="6"/>
+        <v>0.43437637289540937</v>
+      </c>
+      <c r="J18" s="9">
+        <f t="shared" si="0"/>
+        <v>0.75622850667309949</v>
+      </c>
+      <c r="K18" s="9">
+        <f t="shared" si="1"/>
+        <v>0.85041452621941915</v>
+      </c>
+      <c r="M18" s="9">
+        <f t="shared" si="7"/>
+        <v>0.5506400602409639</v>
+      </c>
+      <c r="N18" s="9">
+        <f t="shared" si="2"/>
+        <v>1.03639690618609</v>
+      </c>
+      <c r="O18" s="9">
+        <f t="shared" si="3"/>
+        <v>1.2897651886821562</v>
+      </c>
+      <c r="Q18" s="9">
+        <f t="shared" si="8"/>
         <v>1.7409522107114854</v>
       </c>
-      <c r="J18" s="9">
-        <f>(G18/G$74)/($E18/F$74)</f>
-        <v>0.71979553913670524</v>
-      </c>
-      <c r="L18" s="9">
-        <f>IF($C18&lt;&gt;"", (F18/F$75)/($E18/E$75), "")</f>
-        <v>1.8821676463796617</v>
-      </c>
-      <c r="M18" s="9">
-        <f>IF($C18&lt;&gt;"", (G18/G$75)/($E18/F$75), "")</f>
-        <v>0.79655555095504915</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="R18" s="9">
+        <f t="shared" si="4"/>
+        <v>1.9577826495277286</v>
+      </c>
+      <c r="T18" s="9">
+        <f t="shared" si="9"/>
+        <v>1.8821676463796615</v>
+      </c>
+      <c r="U18" s="9">
+        <f t="shared" si="5"/>
+        <v>2.342301771719526</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>188</v>
       </c>
@@ -2180,23 +2634,47 @@
         <v>294</v>
       </c>
       <c r="I19" s="9">
-        <f>(F19/F$74)/($E19/E$74)</f>
-        <v>0.85314733381931851</v>
+        <f t="shared" si="6"/>
+        <v>0.27617757042115532</v>
       </c>
       <c r="J19" s="9">
-        <f>(G19/G$74)/($E19/F$74)</f>
-        <v>0.39813283246624009</v>
-      </c>
-      <c r="L19" s="9">
-        <f>IF($C19&lt;&gt;"", (F19/F$75)/($E19/E$75), "")</f>
-        <v>0.9223494472910041</v>
+        <f t="shared" si="0"/>
+        <v>0.23562015786550577</v>
+      </c>
+      <c r="K19" s="9">
+        <f t="shared" si="1"/>
+        <v>0.29906922333553737</v>
       </c>
       <c r="M19" s="9">
-        <f>IF($C19&lt;&gt;"", (G19/G$75)/($E19/F$75), "")</f>
-        <v>0.44059027942684864</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0.35009830990629182</v>
+      </c>
+      <c r="N19" s="9">
+        <f t="shared" si="2"/>
+        <v>0.32291298263958296</v>
+      </c>
+      <c r="O19" s="9">
+        <f t="shared" si="3"/>
+        <v>0.45357770989539942</v>
+      </c>
+      <c r="Q19" s="9">
+        <f t="shared" si="8"/>
+        <v>0.85314733381931862</v>
+      </c>
+      <c r="R19" s="9">
+        <f t="shared" si="4"/>
+        <v>1.082887444043604</v>
+      </c>
+      <c r="T19" s="9">
+        <f t="shared" si="9"/>
+        <v>0.92234944729100421</v>
+      </c>
+      <c r="U19" s="9">
+        <f t="shared" si="5"/>
+        <v>1.2955724065529055</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>188</v>
       </c>
@@ -2219,23 +2697,47 @@
         <v>102</v>
       </c>
       <c r="I20" s="9">
-        <f>(F20/F$74)/($E20/E$74)</f>
-        <v>0.6390161635022753</v>
+        <f t="shared" si="6"/>
+        <v>6.8477186990159492E-2</v>
       </c>
       <c r="J20" s="9">
-        <f>(G20/G$74)/($E20/F$74)</f>
-        <v>0.55708739030175947</v>
-      </c>
-      <c r="L20" s="9">
-        <f>IF($C20&lt;&gt;"", (F20/F$75)/($E20/E$75), "")</f>
-        <v>0.6908492611443422</v>
+        <f t="shared" si="0"/>
+        <v>4.3758029317879643E-2</v>
+      </c>
+      <c r="K20" s="9">
+        <f t="shared" si="1"/>
+        <v>0.10375871013681909</v>
       </c>
       <c r="M20" s="9">
-        <f>IF($C20&lt;&gt;"", (G20/G$75)/($E20/F$75), "")</f>
-        <v>0.6164959755712659</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>8.6805555555555552E-2</v>
+      </c>
+      <c r="N20" s="9">
+        <f t="shared" si="2"/>
+        <v>5.9969553918779693E-2</v>
+      </c>
+      <c r="O20" s="9">
+        <f t="shared" si="3"/>
+        <v>0.15736369526983246</v>
+      </c>
+      <c r="Q20" s="9">
+        <f t="shared" si="8"/>
+        <v>0.63901616350227541</v>
+      </c>
+      <c r="R20" s="9">
+        <f t="shared" si="4"/>
+        <v>1.5152303226435064</v>
+      </c>
+      <c r="T20" s="9">
+        <f t="shared" si="9"/>
+        <v>0.69084926114434209</v>
+      </c>
+      <c r="U20" s="9">
+        <f t="shared" si="5"/>
+        <v>1.8128297695084701</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>188</v>
       </c>
@@ -2253,23 +2755,38 @@
         <v>367</v>
       </c>
       <c r="I21" s="9">
-        <f>(F21/F$74)/($E21/E$74)</f>
+        <f t="shared" si="6"/>
+        <v>0.30154713066148547</v>
+      </c>
+      <c r="J21" s="9">
+        <f t="shared" si="0"/>
+        <v>0.31584321161495177</v>
+      </c>
+      <c r="K21" s="9">
+        <f t="shared" si="1"/>
+        <v>0.37332790804130006</v>
+      </c>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="Q21" s="9">
+        <f t="shared" si="8"/>
         <v>1.047409109554801</v>
       </c>
-      <c r="J21" s="9">
-        <f>(G21/G$74)/($E21/F$74)</f>
-        <v>0.45517660459703047</v>
-      </c>
-      <c r="L21" s="9" t="str">
-        <f>IF($C21&lt;&gt;"", (F21/F$75)/($E21/E$75), "")</f>
+      <c r="R21" s="9">
+        <f t="shared" si="4"/>
+        <v>1.2380416528001892</v>
+      </c>
+      <c r="T21" s="9" t="str">
+        <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="M21" s="9" t="str">
-        <f>IF($C21&lt;&gt;"", (G21/G$75)/($E21/F$75), "")</f>
+      <c r="U21" s="9" t="str">
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>189</v>
       </c>
@@ -2292,23 +2809,47 @@
         <v>16</v>
       </c>
       <c r="I22" s="9">
-        <f>(F22/F$74)/($E22/E$74)</f>
+        <f t="shared" si="6"/>
+        <v>3.3001053971161206E-3</v>
+      </c>
+      <c r="J22" s="9">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J22" s="9">
-        <f>(G22/G$74)/($E22/F$74)</f>
-        <v>1.813264839021413</v>
-      </c>
-      <c r="L22" s="9">
-        <f>IF($C22&lt;&gt;"", (F22/F$75)/($E22/E$75), "")</f>
+      <c r="K22" s="9">
+        <f t="shared" si="1"/>
+        <v>1.6275876099893189E-2</v>
+      </c>
+      <c r="M22" s="9">
+        <f t="shared" si="7"/>
+        <v>4.1834002677376171E-3</v>
+      </c>
+      <c r="N22" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M22" s="9">
-        <f>IF($C22&lt;&gt;"", (G22/G$75)/($E22/F$75), "")</f>
-        <v>2.0066339597025515</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O22" s="9">
+        <f t="shared" si="3"/>
+        <v>2.4684501218797249E-2</v>
+      </c>
+      <c r="Q22" s="9">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="R22" s="9">
+        <f t="shared" si="4"/>
+        <v>4.9319261482121961</v>
+      </c>
+      <c r="T22" s="9">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U22" s="9">
+        <f t="shared" si="5"/>
+        <v>5.9005831713412942</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>189</v>
       </c>
@@ -2330,23 +2871,47 @@
         <v>155</v>
       </c>
       <c r="I23" s="9">
-        <f>(F23/F$74)/($E23/E$74)</f>
-        <v>0.27238061039200462</v>
+        <f t="shared" si="6"/>
+        <v>0.43252006360953155</v>
       </c>
       <c r="J23" s="9">
-        <f>(G23/G$74)/($E23/F$74)</f>
-        <v>0.13402768242647545</v>
-      </c>
-      <c r="L23" s="9">
-        <f>IF($C23&lt;&gt;"", (F23/F$75)/($E23/E$75), "")</f>
+        <f t="shared" si="0"/>
+        <v>0.11781007893275289</v>
+      </c>
+      <c r="K23" s="9">
+        <f t="shared" si="1"/>
+        <v>0.15767254971771527</v>
+      </c>
+      <c r="M23" s="9">
+        <f t="shared" si="7"/>
+        <v>0.54828689759036142</v>
+      </c>
+      <c r="N23" s="9">
+        <f t="shared" si="2"/>
+        <v>0.16145649131979148</v>
+      </c>
+      <c r="O23" s="9">
+        <f t="shared" si="3"/>
+        <v>0.23913110555709835</v>
+      </c>
+      <c r="Q23" s="9">
+        <f t="shared" si="8"/>
+        <v>0.27238061039200467</v>
+      </c>
+      <c r="R23" s="9">
+        <f t="shared" si="4"/>
+        <v>0.3645438974596521</v>
+      </c>
+      <c r="T23" s="9">
+        <f t="shared" si="9"/>
         <v>0.29447446588523002</v>
       </c>
-      <c r="M23" s="9">
-        <f>IF($C23&lt;&gt;"", (G23/G$75)/($E23/F$75), "")</f>
-        <v>0.14832058357362687</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="U23" s="9">
+        <f t="shared" si="5"/>
+        <v>0.43614229449589925</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>189</v>
       </c>
@@ -2366,23 +2931,47 @@
         <v>25</v>
       </c>
       <c r="I24" s="9">
-        <f>(F24/F$74)/($E24/E$74)</f>
-        <v>0.55839313591148054</v>
+        <f t="shared" si="6"/>
+        <v>0.15572372342641694</v>
       </c>
       <c r="J24" s="9">
-        <f>(G24/G$74)/($E24/F$74)</f>
-        <v>6.0041882086801744E-2</v>
-      </c>
-      <c r="L24" s="9">
-        <f>IF($C24&lt;&gt;"", (F24/F$75)/($E24/E$75), "")</f>
-        <v>0.60368658479347681</v>
+        <f t="shared" si="0"/>
+        <v>8.6955058259889029E-2</v>
+      </c>
+      <c r="K24" s="9">
+        <f t="shared" si="1"/>
+        <v>2.5431056406083109E-2</v>
       </c>
       <c r="M24" s="9">
-        <f>IF($C24&lt;&gt;"", (G24/G$75)/($E24/F$75), "")</f>
-        <v>6.6444833102733497E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0.19740420013386881</v>
+      </c>
+      <c r="N24" s="9">
+        <f t="shared" si="2"/>
+        <v>0.11917026740270324</v>
+      </c>
+      <c r="O24" s="9">
+        <f t="shared" si="3"/>
+        <v>3.85695331543707E-2</v>
+      </c>
+      <c r="Q24" s="9">
+        <f t="shared" si="8"/>
+        <v>0.55839313591148043</v>
+      </c>
+      <c r="R24" s="9">
+        <f t="shared" si="4"/>
+        <v>0.1633088128547085</v>
+      </c>
+      <c r="T24" s="9">
+        <f t="shared" si="9"/>
+        <v>0.6036865847934767</v>
+      </c>
+      <c r="U24" s="9">
+        <f t="shared" si="5"/>
+        <v>0.1953835487199104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>189</v>
       </c>
@@ -2403,23 +2992,47 @@
         <v>0</v>
       </c>
       <c r="I25" s="9">
-        <f>(F25/F$74)/($E25/E$74)</f>
-        <v>1.5358140463661005</v>
+        <f t="shared" si="6"/>
+        <v>4.7851528258183743E-2</v>
       </c>
       <c r="J25" s="9">
-        <f>(G25/G$74)/($E25/F$74)</f>
+        <f t="shared" si="0"/>
+        <v>7.3491049239002987E-2</v>
+      </c>
+      <c r="K25" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L25" s="9">
-        <f>IF($C25&lt;&gt;"", (F25/F$75)/($E25/E$75), "")</f>
+      <c r="M25" s="9">
+        <f t="shared" si="7"/>
+        <v>6.0659303882195446E-2</v>
+      </c>
+      <c r="N25" s="9">
+        <f t="shared" si="2"/>
+        <v>0.10071809696615565</v>
+      </c>
+      <c r="O25" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q25" s="9">
+        <f t="shared" si="8"/>
+        <v>1.5358140463661007</v>
+      </c>
+      <c r="R25" s="9">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="T25" s="9">
+        <f t="shared" si="9"/>
         <v>1.6603899240544722</v>
       </c>
-      <c r="M25" s="9">
-        <f>IF($C25&lt;&gt;"", (G25/G$75)/($E25/F$75), "")</f>
+      <c r="U25" s="9">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>189</v>
       </c>
@@ -2439,23 +3052,47 @@
         <v>53</v>
       </c>
       <c r="I26" s="9">
-        <f>(F26/F$74)/($E26/E$74)</f>
+        <f t="shared" si="6"/>
+        <v>1.8150579684138662E-2</v>
+      </c>
+      <c r="J26" s="9">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J26" s="9">
-        <f>(G26/G$74)/($E26/F$74)</f>
-        <v>1.0920799598651689</v>
-      </c>
-      <c r="L26" s="9">
-        <f>IF($C26&lt;&gt;"", (F26/F$75)/($E26/E$75), "")</f>
+      <c r="K26" s="9">
+        <f t="shared" si="1"/>
+        <v>5.391383958089619E-2</v>
+      </c>
+      <c r="M26" s="9">
+        <f t="shared" si="7"/>
+        <v>2.3008701472556896E-2</v>
+      </c>
+      <c r="N26" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M26" s="9">
-        <f>IF($C26&lt;&gt;"", (G26/G$75)/($E26/F$75), "")</f>
-        <v>1.2085409075481277</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O26" s="9">
+        <f t="shared" si="3"/>
+        <v>8.1767410287265876E-2</v>
+      </c>
+      <c r="Q26" s="9">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="R26" s="9">
+        <f t="shared" si="4"/>
+        <v>2.9703646119914366</v>
+      </c>
+      <c r="T26" s="9">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U26" s="9">
+        <f t="shared" si="5"/>
+        <v>3.5537603191032789</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>189</v>
       </c>
@@ -2477,23 +3114,47 @@
         <v>518</v>
       </c>
       <c r="I27" s="9">
-        <f>(F27/F$74)/($E27/E$74)</f>
+        <f t="shared" si="6"/>
+        <v>8.6421510086978404E-2</v>
+      </c>
+      <c r="J27" s="9">
+        <f t="shared" si="0"/>
+        <v>1.5926800670956449</v>
+      </c>
+      <c r="K27" s="9">
+        <f t="shared" si="1"/>
+        <v>0.52693148873404205</v>
+      </c>
+      <c r="M27" s="9">
+        <f t="shared" si="7"/>
+        <v>0.10955279451137885</v>
+      </c>
+      <c r="N27" s="9">
+        <f t="shared" si="2"/>
+        <v>2.1827379945566099</v>
+      </c>
+      <c r="O27" s="9">
+        <f t="shared" si="3"/>
+        <v>0.79916072695856089</v>
+      </c>
+      <c r="Q27" s="9">
+        <f t="shared" si="8"/>
         <v>18.429208949169041</v>
       </c>
-      <c r="J27" s="9">
-        <f>(G27/G$74)/($E27/F$74)</f>
-        <v>2.2416973427520093</v>
-      </c>
-      <c r="L27" s="9">
-        <f>IF($C27&lt;&gt;"", (F27/F$75)/($E27/E$75), "")</f>
+      <c r="R27" s="9">
+        <f t="shared" si="4"/>
+        <v>6.0972261211788021</v>
+      </c>
+      <c r="T27" s="9">
+        <f t="shared" si="9"/>
         <v>19.924074089501175</v>
       </c>
-      <c r="M27" s="9">
-        <f>IF($C27&lt;&gt;"", (G27/G$75)/($E27/F$75), "")</f>
-        <v>2.4807551100857319</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="U27" s="9">
+        <f t="shared" si="5"/>
+        <v>7.2947543741164447</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>189</v>
       </c>
@@ -2516,23 +3177,47 @@
         <v>89</v>
       </c>
       <c r="I28" s="9">
-        <f>(F28/F$74)/($E28/E$74)</f>
-        <v>9.2211750823336464E-2</v>
+        <f t="shared" si="6"/>
+        <v>1.6913040160220116</v>
       </c>
       <c r="J28" s="9">
-        <f>(G28/G$74)/($E28/F$74)</f>
-        <v>1.9680557399134848E-2</v>
-      </c>
-      <c r="L28" s="9">
-        <f>IF($C28&lt;&gt;"", (F28/F$75)/($E28/E$75), "")</f>
+        <f t="shared" si="0"/>
+        <v>0.15595810449193001</v>
+      </c>
+      <c r="K28" s="9">
+        <f t="shared" si="1"/>
+        <v>9.0534560805655862E-2</v>
+      </c>
+      <c r="M28" s="9">
+        <f t="shared" si="7"/>
+        <v>2.1439926372155287</v>
+      </c>
+      <c r="N28" s="9">
+        <f t="shared" si="2"/>
+        <v>0.21373764089000968</v>
+      </c>
+      <c r="O28" s="9">
+        <f t="shared" si="3"/>
+        <v>0.13730753802955969</v>
+      </c>
+      <c r="Q28" s="9">
+        <f t="shared" si="8"/>
+        <v>9.2211750823336477E-2</v>
+      </c>
+      <c r="R28" s="9">
+        <f t="shared" si="4"/>
+        <v>5.3529442340351889E-2</v>
+      </c>
+      <c r="T28" s="9">
+        <f t="shared" si="9"/>
         <v>9.9691406201654467E-2</v>
       </c>
-      <c r="M28" s="9">
-        <f>IF($C28&lt;&gt;"", (G28/G$75)/($E28/F$75), "")</f>
-        <v>2.1779319806527701E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="U28" s="9">
+        <f t="shared" si="5"/>
+        <v>6.4042914908460397E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>189</v>
       </c>
@@ -2549,23 +3234,38 @@
         <v>11</v>
       </c>
       <c r="I29" s="9">
-        <f>(F29/F$74)/($E29/E$74)</f>
-        <v>3.6430376028351938</v>
+        <f t="shared" si="6"/>
+        <v>3.4032336907759989E-2</v>
       </c>
       <c r="J29" s="9">
-        <f>(G29/G$74)/($E29/F$74)</f>
-        <v>0.12088432260142754</v>
-      </c>
-      <c r="L29" s="9" t="str">
-        <f>IF($C29&lt;&gt;"", (F29/F$75)/($E29/E$75), "")</f>
+        <f t="shared" si="0"/>
+        <v>0.12398108306732565</v>
+      </c>
+      <c r="K29" s="9">
+        <f t="shared" si="1"/>
+        <v>1.1189664818676568E-2</v>
+      </c>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+      <c r="Q29" s="9">
+        <f t="shared" si="8"/>
+        <v>3.6430376028351943</v>
+      </c>
+      <c r="R29" s="9">
+        <f t="shared" si="4"/>
+        <v>0.3287950765474798</v>
+      </c>
+      <c r="T29" s="9" t="str">
+        <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="M29" s="9" t="str">
-        <f>IF($C29&lt;&gt;"", (G29/G$75)/($E29/F$75), "")</f>
+      <c r="U29" s="9" t="str">
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>190</v>
       </c>
@@ -2588,23 +3288,47 @@
         <v>18</v>
       </c>
       <c r="I30" s="9">
-        <f>(F30/F$74)/($E30/E$74)</f>
+        <f t="shared" si="6"/>
+        <v>0.24028892422751752</v>
+      </c>
+      <c r="J30" s="9">
+        <f t="shared" si="0"/>
+        <v>3.8148025559177123E-2</v>
+      </c>
+      <c r="K30" s="9">
+        <f t="shared" si="1"/>
+        <v>1.8310360612379839E-2</v>
+      </c>
+      <c r="M30" s="9">
+        <f t="shared" si="7"/>
+        <v>0.30460383199464525</v>
+      </c>
+      <c r="N30" s="9">
+        <f t="shared" si="2"/>
+        <v>5.2281149570218198E-2</v>
+      </c>
+      <c r="O30" s="9">
+        <f t="shared" si="3"/>
+        <v>2.7770063871146902E-2</v>
+      </c>
+      <c r="Q30" s="9">
+        <f t="shared" si="8"/>
         <v>0.15875898434276842</v>
       </c>
-      <c r="J30" s="9">
-        <f>(G30/G$74)/($E30/F$74)</f>
-        <v>2.801610910076003E-2</v>
-      </c>
-      <c r="L30" s="9">
-        <f>IF($C30&lt;&gt;"", (F30/F$75)/($E30/E$75), "")</f>
+      <c r="R30" s="9">
+        <f t="shared" si="4"/>
+        <v>7.6201434049630506E-2</v>
+      </c>
+      <c r="T30" s="9">
+        <f t="shared" si="9"/>
         <v>0.17163654583024834</v>
       </c>
-      <c r="M30" s="9">
-        <f>IF($C30&lt;&gt;"", (G30/G$75)/($E30/F$75), "")</f>
-        <v>3.1003786501842004E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="U30" s="9">
+        <f t="shared" si="5"/>
+        <v>9.116780865591699E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>190</v>
       </c>
@@ -2627,23 +3351,47 @@
         <v>1689</v>
       </c>
       <c r="I31" s="9">
-        <f>(F31/F$74)/($E31/E$74)</f>
+        <f t="shared" si="6"/>
+        <v>0.22172583136873933</v>
+      </c>
+      <c r="J31" s="9">
+        <f t="shared" si="0"/>
+        <v>9.6621094736133468</v>
+      </c>
+      <c r="K31" s="9">
+        <f t="shared" si="1"/>
+        <v>1.7181221707949748</v>
+      </c>
+      <c r="M31" s="9">
+        <f t="shared" si="7"/>
+        <v>0.28107220548862116</v>
+      </c>
+      <c r="N31" s="9">
+        <f t="shared" si="2"/>
+        <v>13.241738809527471</v>
+      </c>
+      <c r="O31" s="9">
+        <f t="shared" si="3"/>
+        <v>2.6057576599092847</v>
+      </c>
+      <c r="Q31" s="9">
+        <f t="shared" si="8"/>
         <v>43.576832766701209</v>
       </c>
-      <c r="J31" s="9">
-        <f>(G31/G$74)/($E31/F$74)</f>
-        <v>2.8489342447508528</v>
-      </c>
-      <c r="L31" s="9">
-        <f>IF($C31&lt;&gt;"", (F31/F$75)/($E31/E$75), "")</f>
-        <v>47.111519926019675</v>
-      </c>
-      <c r="M31" s="9">
-        <f>IF($C31&lt;&gt;"", (G31/G$75)/($E31/F$75), "")</f>
-        <v>3.1527486120349861</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="R31" s="9">
+        <f t="shared" si="4"/>
+        <v>7.7488588505399072</v>
+      </c>
+      <c r="T31" s="9">
+        <f t="shared" si="9"/>
+        <v>47.111519926019668</v>
+      </c>
+      <c r="U31" s="9">
+        <f t="shared" si="5"/>
+        <v>9.2707767222283213</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>190</v>
       </c>
@@ -2666,23 +3414,47 @@
         <v>223</v>
       </c>
       <c r="I32" s="9">
-        <f>(F32/F$74)/($E32/E$74)</f>
+        <f t="shared" si="6"/>
+        <v>1.5743565310117091</v>
+      </c>
+      <c r="J32" s="9">
+        <f t="shared" si="0"/>
+        <v>0.18793512591653436</v>
+      </c>
+      <c r="K32" s="9">
+        <f t="shared" si="1"/>
+        <v>0.22684502314226132</v>
+      </c>
+      <c r="M32" s="9">
+        <f t="shared" si="7"/>
+        <v>1.995743390227577</v>
+      </c>
+      <c r="N32" s="9">
+        <f t="shared" si="2"/>
+        <v>0.25756154567681022</v>
+      </c>
+      <c r="O32" s="9">
+        <f t="shared" si="3"/>
+        <v>0.34404023573698667</v>
+      </c>
+      <c r="Q32" s="9">
+        <f t="shared" si="8"/>
         <v>0.11937265937834549</v>
       </c>
-      <c r="J32" s="9">
-        <f>(G32/G$74)/($E32/F$74)</f>
-        <v>5.2974984816163376E-2</v>
-      </c>
-      <c r="L32" s="9">
-        <f>IF($C32&lt;&gt;"", (F32/F$75)/($E32/E$75), "")</f>
+      <c r="R32" s="9">
+        <f t="shared" si="4"/>
+        <v>0.14408745330162712</v>
+      </c>
+      <c r="T32" s="9">
+        <f t="shared" si="9"/>
         <v>0.1290554421665604</v>
       </c>
-      <c r="M32" s="9">
-        <f>IF($C32&lt;&gt;"", (G32/G$75)/($E32/F$75), "")</f>
-        <v>5.8624311936809781E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="U32" s="9">
+        <f t="shared" si="5"/>
+        <v>0.17238700998416201</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>190</v>
       </c>
@@ -2705,23 +3477,47 @@
         <v>25</v>
       </c>
       <c r="I33" s="9">
-        <f>(F33/F$74)/($E33/E$74)</f>
+        <f t="shared" si="6"/>
+        <v>5.0359608359991999</v>
+      </c>
+      <c r="J33" s="9">
+        <f t="shared" si="0"/>
+        <v>0.14810409922974649</v>
+      </c>
+      <c r="K33" s="9">
+        <f t="shared" si="1"/>
+        <v>2.5431056406083109E-2</v>
+      </c>
+      <c r="M33" s="9">
+        <f t="shared" si="7"/>
+        <v>6.3838688085676036</v>
+      </c>
+      <c r="N33" s="9">
+        <f t="shared" si="2"/>
+        <v>0.20297387480202359</v>
+      </c>
+      <c r="O33" s="9">
+        <f t="shared" si="3"/>
+        <v>3.85695331543707E-2</v>
+      </c>
+      <c r="Q33" s="9">
+        <f t="shared" si="8"/>
         <v>2.9409303219960551E-2</v>
       </c>
-      <c r="J33" s="9">
-        <f>(G33/G$74)/($E33/F$74)</f>
-        <v>1.8566358525366694E-3</v>
-      </c>
-      <c r="L33" s="9">
-        <f>IF($C33&lt;&gt;"", (F33/F$75)/($E33/E$75), "")</f>
-        <v>3.17948067055542E-2</v>
-      </c>
-      <c r="M33" s="9">
-        <f>IF($C33&lt;&gt;"", (G33/G$75)/($E33/F$75), "")</f>
-        <v>2.0546301192891463E-3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="R33" s="9">
+        <f t="shared" si="4"/>
+        <v>5.0498916163706142E-3</v>
+      </c>
+      <c r="T33" s="9">
+        <f t="shared" si="9"/>
+        <v>3.1794806705554207E-2</v>
+      </c>
+      <c r="U33" s="9">
+        <f t="shared" si="5"/>
+        <v>6.041717696737072E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>190</v>
       </c>
@@ -2744,23 +3540,47 @@
         <v>2751</v>
       </c>
       <c r="I34" s="9">
-        <f>(F34/F$74)/($E34/E$74)</f>
+        <f t="shared" si="6"/>
+        <v>1.084497136127285</v>
+      </c>
+      <c r="J34" s="9">
+        <f t="shared" si="0"/>
+        <v>5.3659685951989591</v>
+      </c>
+      <c r="K34" s="9">
+        <f t="shared" si="1"/>
+        <v>2.7984334469253853</v>
+      </c>
+      <c r="M34" s="9">
+        <f t="shared" si="7"/>
+        <v>1.3747699129852744</v>
+      </c>
+      <c r="N34" s="9">
+        <f t="shared" si="2"/>
+        <v>7.3539587593990747</v>
+      </c>
+      <c r="O34" s="9">
+        <f t="shared" si="3"/>
+        <v>4.2441914283069515</v>
+      </c>
+      <c r="Q34" s="9">
+        <f t="shared" si="8"/>
         <v>4.9478863672805193</v>
       </c>
-      <c r="J34" s="9">
-        <f>(G34/G$74)/($E34/F$74)</f>
-        <v>0.9487051297352429</v>
-      </c>
-      <c r="L34" s="9">
-        <f>IF($C34&lt;&gt;"", (F34/F$75)/($E34/E$75), "")</f>
-        <v>5.3492287618006999</v>
-      </c>
-      <c r="M34" s="9">
-        <f>IF($C34&lt;&gt;"", (G34/G$75)/($E34/F$75), "")</f>
-        <v>1.0498763832525142</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="R34" s="9">
+        <f t="shared" si="4"/>
+        <v>2.58039726773141</v>
+      </c>
+      <c r="T34" s="9">
+        <f t="shared" si="9"/>
+        <v>5.3492287618006991</v>
+      </c>
+      <c r="U34" s="9">
+        <f t="shared" si="5"/>
+        <v>3.0872012750779572</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>190</v>
       </c>
@@ -2783,23 +3603,47 @@
         <v>4560</v>
       </c>
       <c r="I35" s="9">
-        <f>(F35/F$74)/($E35/E$74)</f>
-        <v>0.44824122245568915</v>
+        <f t="shared" si="6"/>
+        <v>8.2490259532663828</v>
       </c>
       <c r="J35" s="9">
-        <f>(G35/G$74)/($E35/F$74)</f>
-        <v>0.20674320312891045</v>
-      </c>
-      <c r="L35" s="9">
-        <f>IF($C35&lt;&gt;"", (F35/F$75)/($E35/E$75), "")</f>
-        <v>0.48459981927647583</v>
+        <f t="shared" si="0"/>
+        <v>3.6975534773608296</v>
+      </c>
+      <c r="K35" s="9">
+        <f t="shared" si="1"/>
+        <v>4.6386246884695588</v>
       </c>
       <c r="M35" s="9">
-        <f>IF($C35&lt;&gt;"", (G35/G$75)/($E35/F$75), "")</f>
-        <v>0.22879058999459009</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>10.456931894243642</v>
+      </c>
+      <c r="N35" s="9">
+        <f t="shared" si="2"/>
+        <v>5.0674273061368842</v>
+      </c>
+      <c r="O35" s="9">
+        <f t="shared" si="3"/>
+        <v>7.0350828473572156</v>
+      </c>
+      <c r="Q35" s="9">
+        <f t="shared" si="8"/>
+        <v>0.44824122245568909</v>
+      </c>
+      <c r="R35" s="9">
+        <f t="shared" si="4"/>
+        <v>0.56232392948561327</v>
+      </c>
+      <c r="T35" s="9">
+        <f t="shared" si="9"/>
+        <v>0.48459981927647577</v>
+      </c>
+      <c r="U35" s="9">
+        <f t="shared" si="5"/>
+        <v>0.67276739664240381</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>190</v>
       </c>
@@ -2818,23 +3662,38 @@
         <v>1959</v>
       </c>
       <c r="I36" s="9">
-        <f>(F36/F$74)/($E36/E$74)</f>
+        <f t="shared" si="6"/>
+        <v>1.9072546629457978</v>
+      </c>
+      <c r="J36" s="9">
+        <f t="shared" si="0"/>
+        <v>1.9601353132906598</v>
+      </c>
+      <c r="K36" s="9">
+        <f t="shared" si="1"/>
+        <v>1.9927775799806724</v>
+      </c>
+      <c r="M36" s="9"/>
+      <c r="N36" s="9"/>
+      <c r="O36" s="9"/>
+      <c r="Q36" s="9">
+        <f t="shared" si="8"/>
         <v>1.0277260563952098</v>
       </c>
-      <c r="J36" s="9">
-        <f>(G36/G$74)/($E36/F$74)</f>
-        <v>0.38414467607255842</v>
-      </c>
-      <c r="L36" s="9" t="str">
-        <f>IF($C36&lt;&gt;"", (F36/F$75)/($E36/E$75), "")</f>
+      <c r="R36" s="9">
+        <f t="shared" si="4"/>
+        <v>1.044840848312717</v>
+      </c>
+      <c r="T36" s="9" t="str">
+        <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="M36" s="9" t="str">
-        <f>IF($C36&lt;&gt;"", (G36/G$75)/($E36/F$75), "")</f>
+      <c r="U36" s="9" t="str">
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>191</v>
       </c>
@@ -2859,23 +3718,47 @@
         <v>352</v>
       </c>
       <c r="I37" s="9">
-        <f>(F37/F$74)/($E37/E$74)</f>
-        <v>6.7288330777529444</v>
+        <f t="shared" si="6"/>
+        <v>4.7439015083544228E-2</v>
       </c>
       <c r="J37" s="9">
-        <f>(G37/G$74)/($E37/F$74)</f>
-        <v>2.7750835797197277</v>
-      </c>
-      <c r="L37" s="9">
-        <f>IF($C37&lt;&gt;"", (F37/F$75)/($E37/E$75), "")</f>
+        <f t="shared" si="0"/>
+        <v>0.31920921387017331</v>
+      </c>
+      <c r="K37" s="9">
+        <f t="shared" si="1"/>
+        <v>0.35806927419765017</v>
+      </c>
+      <c r="M37" s="9">
+        <f t="shared" si="7"/>
+        <v>6.0136378848728245E-2</v>
+      </c>
+      <c r="N37" s="9">
+        <f t="shared" si="2"/>
+        <v>0.43747020743314935</v>
+      </c>
+      <c r="O37" s="9">
+        <f t="shared" si="3"/>
+        <v>0.54305902681353946</v>
+      </c>
+      <c r="Q37" s="9">
+        <f t="shared" si="8"/>
+        <v>6.7288330777529453</v>
+      </c>
+      <c r="R37" s="9">
+        <f t="shared" si="4"/>
+        <v>7.5479913224812751</v>
+      </c>
+      <c r="T37" s="9">
+        <f t="shared" si="9"/>
         <v>7.2746350180744361</v>
       </c>
-      <c r="M37" s="9">
-        <f>IF($C37&lt;&gt;"", (G37/G$75)/($E37/F$75), "")</f>
-        <v>3.0710224078926012</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="U37" s="9">
+        <f t="shared" si="5"/>
+        <v>9.0304577230962426</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>191</v>
       </c>
@@ -2895,23 +3778,47 @@
         <v>21</v>
       </c>
       <c r="I38" s="9">
-        <f>(F38/F$74)/($E38/E$74)</f>
+        <f t="shared" si="6"/>
+        <v>9.9003161913483618E-3</v>
+      </c>
+      <c r="J38" s="9">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J38" s="9">
-        <f>(G38/G$74)/($E38/F$74)</f>
-        <v>0.79330336707186822</v>
-      </c>
-      <c r="L38" s="9">
-        <f>IF($C38&lt;&gt;"", (F38/F$75)/($E38/E$75), "")</f>
+      <c r="K38" s="9">
+        <f t="shared" si="1"/>
+        <v>2.1362087381109812E-2</v>
+      </c>
+      <c r="M38" s="9">
+        <f t="shared" si="7"/>
+        <v>1.2550200803212851E-2</v>
+      </c>
+      <c r="N38" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M38" s="9">
-        <f>IF($C38&lt;&gt;"", (G38/G$75)/($E38/F$75), "")</f>
-        <v>0.87790235736986644</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O38" s="9">
+        <f t="shared" si="3"/>
+        <v>3.2398407849671386E-2</v>
+      </c>
+      <c r="Q38" s="9">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="R38" s="9">
+        <f t="shared" si="4"/>
+        <v>2.1577176898428361</v>
+      </c>
+      <c r="T38" s="9">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U38" s="9">
+        <f t="shared" si="5"/>
+        <v>2.5815051374618161</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>191</v>
       </c>
@@ -2933,23 +3840,47 @@
         <v>171</v>
       </c>
       <c r="I39" s="9">
-        <f>(F39/F$74)/($E39/E$74)</f>
-        <v>0.41662911310137202</v>
+        <f t="shared" si="6"/>
+        <v>0.30835359804303752</v>
       </c>
       <c r="J39" s="9">
-        <f>(G39/G$74)/($E39/F$74)</f>
-        <v>0.20740353677101112</v>
-      </c>
-      <c r="L39" s="9">
-        <f>IF($C39&lt;&gt;"", (F39/F$75)/($E39/E$75), "")</f>
-        <v>0.45042352822469806</v>
+        <f t="shared" si="0"/>
+        <v>0.12846908607428767</v>
+      </c>
+      <c r="K39" s="9">
+        <f t="shared" si="1"/>
+        <v>0.17394842581760847</v>
       </c>
       <c r="M39" s="9">
-        <f>IF($C39&lt;&gt;"", (G39/G$75)/($E39/F$75), "")</f>
-        <v>0.22952134254791728</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0.39088646251673359</v>
+      </c>
+      <c r="N39" s="9">
+        <f t="shared" si="2"/>
+        <v>0.17606445958205835</v>
+      </c>
+      <c r="O39" s="9">
+        <f t="shared" si="3"/>
+        <v>0.26381560677589561</v>
+      </c>
+      <c r="Q39" s="9">
+        <f t="shared" si="8"/>
+        <v>0.41662911310137196</v>
+      </c>
+      <c r="R39" s="9">
+        <f t="shared" si="4"/>
+        <v>0.56411998083229808</v>
+      </c>
+      <c r="T39" s="9">
+        <f t="shared" si="9"/>
+        <v>0.45042352822469811</v>
+      </c>
+      <c r="U39" s="9">
+        <f t="shared" si="5"/>
+        <v>0.67491620220693072</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>191</v>
       </c>
@@ -2972,23 +3903,47 @@
         <v>235</v>
       </c>
       <c r="I40" s="9">
-        <f>(F40/F$74)/($E40/E$74)</f>
-        <v>1.3061258260730533</v>
+        <f t="shared" si="6"/>
+        <v>0.19800632382696723</v>
       </c>
       <c r="J40" s="9">
-        <f>(G40/G$74)/($E40/F$74)</f>
-        <v>0.44387212205211674</v>
-      </c>
-      <c r="L40" s="9">
-        <f>IF($C40&lt;&gt;"", (F40/F$75)/($E40/E$75), "")</f>
+        <f t="shared" si="0"/>
+        <v>0.25862117327618611</v>
+      </c>
+      <c r="K40" s="9">
+        <f t="shared" si="1"/>
+        <v>0.23905193021718121</v>
+      </c>
+      <c r="M40" s="9">
+        <f t="shared" si="7"/>
+        <v>0.25100401606425704</v>
+      </c>
+      <c r="N40" s="9">
+        <f t="shared" si="2"/>
+        <v>0.35443544046868514</v>
+      </c>
+      <c r="O40" s="9">
+        <f t="shared" si="3"/>
+        <v>0.36255361165108457</v>
+      </c>
+      <c r="Q40" s="9">
+        <f t="shared" si="8"/>
+        <v>1.3061258260730535</v>
+      </c>
+      <c r="R40" s="9">
+        <f t="shared" si="4"/>
+        <v>1.2072944216977772</v>
+      </c>
+      <c r="T40" s="9">
+        <f t="shared" si="9"/>
         <v>1.4120707948272415</v>
       </c>
-      <c r="M40" s="9">
-        <f>IF($C40&lt;&gt;"", (G40/G$75)/($E40/F$75), "")</f>
-        <v>0.49120727138552051</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="U40" s="9">
+        <f t="shared" si="5"/>
+        <v>1.4444135888179208</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>191</v>
       </c>
@@ -3007,23 +3962,38 @@
         <v>302</v>
       </c>
       <c r="I41" s="9">
-        <f>(F41/F$74)/($E41/E$74)</f>
+        <f t="shared" si="6"/>
+        <v>0.1272603143762904</v>
+      </c>
+      <c r="J41" s="9">
+        <f t="shared" si="0"/>
+        <v>0.22215614884461973</v>
+      </c>
+      <c r="K41" s="9">
+        <f t="shared" si="1"/>
+        <v>0.30720716138548393</v>
+      </c>
+      <c r="M41" s="9"/>
+      <c r="N41" s="9"/>
+      <c r="O41" s="9"/>
+      <c r="Q41" s="9">
+        <f t="shared" si="8"/>
         <v>1.7456828543400893</v>
       </c>
-      <c r="J41" s="9">
-        <f>(G41/G$74)/($E41/F$74)</f>
-        <v>0.88752995362150189</v>
-      </c>
-      <c r="L41" s="9" t="str">
-        <f>IF($C41&lt;&gt;"", (F41/F$75)/($E41/E$75), "")</f>
+      <c r="R41" s="9">
+        <f t="shared" si="4"/>
+        <v>2.4140059915074281</v>
+      </c>
+      <c r="T41" s="9" t="str">
+        <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="M41" s="9" t="str">
-        <f>IF($C41&lt;&gt;"", (G41/G$75)/($E41/F$75), "")</f>
+      <c r="U41" s="9" t="str">
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>192</v>
       </c>
@@ -3049,23 +4019,47 @@
         <v>1041</v>
       </c>
       <c r="I42" s="9">
-        <f>(F42/F$74)/($E42/E$74)</f>
+        <f t="shared" si="6"/>
+        <v>5.8878005416297983</v>
+      </c>
+      <c r="J42" s="9">
+        <f t="shared" si="0"/>
+        <v>2.5626497169753102</v>
+      </c>
+      <c r="K42" s="9">
+        <f t="shared" si="1"/>
+        <v>1.0589491887493006</v>
+      </c>
+      <c r="M42" s="9">
+        <f t="shared" si="7"/>
+        <v>7.4637090026773762</v>
+      </c>
+      <c r="N42" s="9">
+        <f t="shared" si="2"/>
+        <v>3.5120631064228931</v>
+      </c>
+      <c r="O42" s="9">
+        <f t="shared" si="3"/>
+        <v>1.606035360547996</v>
+      </c>
+      <c r="Q42" s="9">
+        <f t="shared" si="8"/>
         <v>0.43524737274234238</v>
       </c>
-      <c r="J42" s="9">
-        <f>(G42/G$74)/($E42/F$74)</f>
-        <v>6.6125155798405749E-2</v>
-      </c>
-      <c r="L42" s="9">
-        <f>IF($C42&lt;&gt;"", (F42/F$75)/($E42/E$75), "")</f>
-        <v>0.47055198764622896</v>
-      </c>
-      <c r="M42" s="9">
-        <f>IF($C42&lt;&gt;"", (G42/G$75)/($E42/F$75), "")</f>
-        <v>7.3176835705540413E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="R42" s="9">
+        <f t="shared" si="4"/>
+        <v>0.17985479998209544</v>
+      </c>
+      <c r="T42" s="9">
+        <f t="shared" si="9"/>
+        <v>0.47055198764622902</v>
+      </c>
+      <c r="U42" s="9">
+        <f t="shared" si="5"/>
+        <v>0.21517925738689439</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>192</v>
       </c>
@@ -3087,23 +4081,47 @@
         <v>656</v>
       </c>
       <c r="I43" s="9">
-        <f>(F43/F$74)/($E43/E$74)</f>
+        <f t="shared" si="6"/>
+        <v>0.10354080683451827</v>
+      </c>
+      <c r="J43" s="9">
+        <f t="shared" si="0"/>
+        <v>0.21037514095134444</v>
+      </c>
+      <c r="K43" s="9">
+        <f t="shared" si="1"/>
+        <v>0.66731092009562076</v>
+      </c>
+      <c r="M43" s="9">
+        <f t="shared" si="7"/>
+        <v>0.13125418340026773</v>
+      </c>
+      <c r="N43" s="9">
+        <f t="shared" si="2"/>
+        <v>0.28831516307105626</v>
+      </c>
+      <c r="O43" s="9">
+        <f t="shared" si="3"/>
+        <v>1.0120645499706871</v>
+      </c>
+      <c r="Q43" s="9">
+        <f t="shared" si="8"/>
         <v>2.031808978343888</v>
       </c>
-      <c r="J43" s="9">
-        <f>(G43/G$74)/($E43/F$74)</f>
-        <v>2.3695253673267866</v>
-      </c>
-      <c r="L43" s="9">
-        <f>IF($C43&lt;&gt;"", (F43/F$75)/($E43/E$75), "")</f>
+      <c r="R43" s="9">
+        <f t="shared" si="4"/>
+        <v>6.4449074765482095</v>
+      </c>
+      <c r="T43" s="9">
+        <f t="shared" si="9"/>
         <v>2.1966169428049493</v>
       </c>
-      <c r="M43" s="9">
-        <f>IF($C43&lt;&gt;"", (G43/G$75)/($E43/F$75), "")</f>
-        <v>2.6222148955475579</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="U43" s="9">
+        <f t="shared" si="5"/>
+        <v>7.7107222318722881</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>192</v>
       </c>
@@ -3126,23 +4144,47 @@
         <v>186</v>
       </c>
       <c r="I44" s="9">
-        <f>(F44/F$74)/($E44/E$74)</f>
-        <v>0.56064615801327056</v>
+        <f t="shared" si="6"/>
+        <v>0.32320407233006004</v>
       </c>
       <c r="J44" s="9">
-        <f>(G44/G$74)/($E44/F$74)</f>
-        <v>0.2152311806368748</v>
-      </c>
-      <c r="L44" s="9">
-        <f>IF($C44&lt;&gt;"", (F44/F$75)/($E44/E$75), "")</f>
+        <f t="shared" si="0"/>
+        <v>0.18120312140609135</v>
+      </c>
+      <c r="K44" s="9">
+        <f t="shared" si="1"/>
+        <v>0.18920705966125834</v>
+      </c>
+      <c r="M44" s="9">
+        <f t="shared" si="7"/>
+        <v>0.40971176372155288</v>
+      </c>
+      <c r="N44" s="9">
+        <f t="shared" si="2"/>
+        <v>0.24833546045853644</v>
+      </c>
+      <c r="O44" s="9">
+        <f t="shared" si="3"/>
+        <v>0.28695732666851803</v>
+      </c>
+      <c r="Q44" s="9">
+        <f t="shared" si="8"/>
+        <v>0.56064615801327045</v>
+      </c>
+      <c r="R44" s="9">
+        <f t="shared" si="4"/>
+        <v>0.58541050642467685</v>
+      </c>
+      <c r="T44" s="9">
+        <f t="shared" si="9"/>
         <v>0.6061223583204447</v>
       </c>
-      <c r="M44" s="9">
-        <f>IF($C44&lt;&gt;"", (G44/G$75)/($E44/F$75), "")</f>
-        <v>0.23818373739928181</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="U44" s="9">
+        <f t="shared" si="5"/>
+        <v>0.70038830240553973</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>192</v>
       </c>
@@ -3161,23 +4203,38 @@
         <v>683</v>
       </c>
       <c r="I45" s="9">
-        <f>(F45/F$74)/($E45/E$74)</f>
-        <v>0.18816642619249474</v>
+        <f t="shared" si="6"/>
+        <v>4.6539736362830091</v>
       </c>
       <c r="J45" s="9">
-        <f>(G45/G$74)/($E45/F$74)</f>
-        <v>5.4886539844514491E-2</v>
-      </c>
-      <c r="L45" s="9" t="str">
-        <f>IF($C45&lt;&gt;"", (F45/F$75)/($E45/E$75), "")</f>
+        <f t="shared" si="0"/>
+        <v>0.87572158673346312</v>
+      </c>
+      <c r="K45" s="9">
+        <f t="shared" si="1"/>
+        <v>0.69477646101419055</v>
+      </c>
+      <c r="M45" s="9"/>
+      <c r="N45" s="9"/>
+      <c r="O45" s="9"/>
+      <c r="Q45" s="9">
+        <f t="shared" si="8"/>
+        <v>0.18816642619249471</v>
+      </c>
+      <c r="R45" s="9">
+        <f t="shared" si="4"/>
+        <v>0.14928672040546578</v>
+      </c>
+      <c r="T45" s="9" t="str">
+        <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="M45" s="9" t="str">
-        <f>IF($C45&lt;&gt;"", (G45/G$75)/($E45/F$75), "")</f>
+      <c r="U45" s="9" t="str">
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>246</v>
       </c>
@@ -3197,23 +4254,47 @@
         <v>8513</v>
       </c>
       <c r="I46" s="9">
-        <f>(F46/F$74)/($E46/E$74)</f>
-        <v>6.2461987427877297</v>
+        <f t="shared" si="6"/>
+        <v>1.5535246156924136</v>
       </c>
       <c r="J46" s="9">
-        <f>(G46/G$74)/($E46/F$74)</f>
-        <v>2.0494322324202452</v>
-      </c>
-      <c r="L46" s="9">
-        <f>IF($C46&lt;&gt;"", (F46/F$75)/($E46/E$75), "")</f>
+        <f t="shared" si="0"/>
+        <v>9.7036235014277459</v>
+      </c>
+      <c r="K46" s="9">
+        <f t="shared" si="1"/>
+        <v>8.6597833273994205</v>
+      </c>
+      <c r="M46" s="9">
+        <f t="shared" si="7"/>
+        <v>1.9693356760374832</v>
+      </c>
+      <c r="N46" s="9">
+        <f t="shared" si="2"/>
+        <v>13.298633001706825</v>
+      </c>
+      <c r="O46" s="9">
+        <f t="shared" si="3"/>
+        <v>13.133697429726311</v>
+      </c>
+      <c r="Q46" s="9">
+        <f t="shared" si="8"/>
+        <v>6.2461987427877306</v>
+      </c>
+      <c r="R46" s="9">
+        <f t="shared" si="4"/>
+        <v>5.574281372773557</v>
+      </c>
+      <c r="T46" s="9">
+        <f t="shared" si="9"/>
         <v>6.7528523265597444</v>
       </c>
-      <c r="M46" s="9">
-        <f>IF($C46&lt;&gt;"", (G46/G$75)/($E46/F$75), "")</f>
-        <v>2.2679865771306189</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="U46" s="9">
+        <f t="shared" si="5"/>
+        <v>6.6691004431264522</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>246</v>
       </c>
@@ -3233,23 +4314,38 @@
         <v>5056</v>
       </c>
       <c r="I47" s="9">
-        <f>(F47/F$74)/($E47/E$74)</f>
-        <v>1.8880814014007457</v>
+        <f t="shared" si="6"/>
+        <v>1.6448962838750663</v>
       </c>
       <c r="J47" s="9">
-        <f>(G47/G$74)/($E47/F$74)</f>
-        <v>1.1495758026447978</v>
-      </c>
-      <c r="L47" s="9" t="str">
-        <f>IF($C47&lt;&gt;"", (F47/F$75)/($E47/E$75), "")</f>
+        <f t="shared" si="0"/>
+        <v>3.1056980808177141</v>
+      </c>
+      <c r="K47" s="9">
+        <f t="shared" si="1"/>
+        <v>5.1431768475662478</v>
+      </c>
+      <c r="M47" s="9"/>
+      <c r="N47" s="9"/>
+      <c r="O47" s="9"/>
+      <c r="Q47" s="9">
+        <f t="shared" si="8"/>
+        <v>1.8880814014007459</v>
+      </c>
+      <c r="R47" s="9">
+        <f t="shared" si="4"/>
+        <v>3.1267484144653124</v>
+      </c>
+      <c r="T47" s="9" t="str">
+        <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="M47" s="9" t="str">
-        <f>IF($C47&lt;&gt;"", (G47/G$75)/($E47/F$75), "")</f>
+      <c r="U47" s="9" t="str">
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>193</v>
       </c>
@@ -3266,34 +4362,50 @@
         <v>10717</v>
       </c>
       <c r="I48" s="9">
-        <f>(F48/F$74)/($E48/E$74)</f>
+        <f t="shared" si="6"/>
+        <v>1.0547961875532399</v>
+      </c>
+      <c r="J48" s="9">
+        <f t="shared" si="0"/>
+        <v>13.615479122371012</v>
+      </c>
+      <c r="K48" s="9">
+        <f t="shared" si="1"/>
+        <v>10.901785260159707</v>
+      </c>
+      <c r="M48" s="9"/>
+      <c r="N48" s="9"/>
+      <c r="O48" s="9"/>
+      <c r="Q48" s="9">
+        <f t="shared" si="8"/>
         <v>12.908161105468333</v>
       </c>
-      <c r="J48" s="9">
-        <f>(G48/G$74)/($E48/F$74)</f>
-        <v>3.7999138208432703</v>
-      </c>
-      <c r="L48" s="9" t="str">
-        <f>IF($C48&lt;&gt;"", (F48/F$75)/($E48/E$75), "")</f>
+      <c r="R48" s="9">
+        <f t="shared" si="4"/>
+        <v>10.335442418926499</v>
+      </c>
+      <c r="T48" s="9" t="str">
+        <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="M48" s="9" t="str">
-        <f>IF($C48&lt;&gt;"", (G48/G$75)/($E48/F$75), "")</f>
+      <c r="U48" s="9" t="str">
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I49" s="9"/>
-      <c r="J49" s="9"/>
-      <c r="L49" s="9"/>
-      <c r="M49" s="9"/>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q49" s="9"/>
+      <c r="R49" s="9"/>
+      <c r="T49" s="9"/>
+      <c r="U49" s="9"/>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I50" s="9"/>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>184</v>
       </c>
@@ -3305,32 +4417,56 @@
         <v>18784</v>
       </c>
       <c r="F51">
-        <f t="shared" ref="F51:G51" si="0">SUMIFS(F$2:F$48,$A$2:$A$48,$A51)-F52</f>
+        <f t="shared" ref="F51:G51" si="10">SUMIFS(F$2:F$48,$A$2:$A$48,$A51)-F52</f>
         <v>19840</v>
       </c>
       <c r="G51">
-        <f t="shared" si="0"/>
+        <f>SUMIFS(G$2:G$48,$A$2:$A$48,$A51)-G52</f>
         <v>10096</v>
       </c>
       <c r="I51" s="9">
-        <f>(F51/F$74)/($E51/$E$74)</f>
+        <f t="shared" si="6"/>
+        <v>3.8743237362143255</v>
+      </c>
+      <c r="J51" s="9">
+        <f t="shared" ref="J51:J69" si="11">100*F51/F$74</f>
+        <v>11.130247457265796</v>
+      </c>
+      <c r="K51" s="9">
+        <f t="shared" ref="K51:K69" si="12">100*G51/G$74</f>
+        <v>10.270077819032602</v>
+      </c>
+      <c r="M51" s="9">
+        <f t="shared" ref="M51:O69" si="13">100*E51/E$75</f>
+        <v>4.9113119143239627</v>
+      </c>
+      <c r="N51" s="9">
+        <f t="shared" si="13"/>
+        <v>15.253794227546015</v>
+      </c>
+      <c r="O51" s="9">
+        <f t="shared" si="13"/>
+        <v>15.575920269061063</v>
+      </c>
+      <c r="Q51" s="9">
+        <f>J51/$I51</f>
         <v>2.8728232886757601</v>
       </c>
-      <c r="J51" s="9">
-        <f>(G51/G$74)/($E51/$E$74)</f>
-        <v>2.6508052806830462</v>
-      </c>
-      <c r="K51" s="9"/>
-      <c r="L51" s="9">
-        <f>IF($D51="", (F51/F$75)/($E51/$E$75), "")</f>
-        <v>3.105849209670017</v>
-      </c>
-      <c r="M51" s="9">
-        <f>IF($D51="", (G51/G$75)/($E51/$E$75), "")</f>
+      <c r="R51" s="9">
+        <f t="shared" ref="R51:R69" si="14">K51/$I51</f>
+        <v>2.6508052806830458</v>
+      </c>
+      <c r="S51" s="9"/>
+      <c r="T51" s="9">
+        <f>IF($D51="", N51/$M51, "")</f>
+        <v>3.1058492096700165</v>
+      </c>
+      <c r="U51" s="9">
+        <f t="shared" ref="U51:U69" si="15">IF($D51="", O51/$M51, "")</f>
         <v>3.1714378033359085</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
         <v>242</v>
       </c>
@@ -3339,32 +4475,44 @@
         <v>1184</v>
       </c>
       <c r="F52">
-        <f t="shared" ref="F52:G52" si="1">SUMIFS(F$2:F$48,$A$2:$A$48,$A51,$D$2:$D$48,"Verkehr")</f>
+        <f t="shared" ref="F52:G52" si="16">SUMIFS(F$2:F$48,$A$2:$A$48,$A51,$D$2:$D$48,"Verkehr")</f>
         <v>634</v>
       </c>
       <c r="G52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>411</v>
       </c>
       <c r="I52" s="9">
-        <f>(F52/F$74)/($E52/$E$74)</f>
+        <f t="shared" si="6"/>
+        <v>0.2442077993865929</v>
+      </c>
+      <c r="J52" s="9">
+        <f t="shared" si="11"/>
+        <v>0.35567423830173966</v>
+      </c>
+      <c r="K52" s="9">
+        <f t="shared" si="12"/>
+        <v>0.4180865673160063</v>
+      </c>
+      <c r="Q52" s="9">
+        <f t="shared" ref="Q52:Q69" si="17">J52/$I52</f>
         <v>1.456440945764758</v>
       </c>
-      <c r="J52" s="9">
-        <f>(G52/G$74)/($E52/$E$74)</f>
-        <v>1.7120115261108215</v>
-      </c>
-      <c r="K52" s="9"/>
-      <c r="L52" s="9" t="str">
-        <f>IF($D52="", (F52/F$75)/($E52/$E$75), "")</f>
+      <c r="R52" s="9">
+        <f t="shared" si="14"/>
+        <v>1.7120115261108217</v>
+      </c>
+      <c r="S52" s="9"/>
+      <c r="T52" s="9" t="str">
+        <f t="shared" ref="T52:T69" si="18">IF($D52="", N52/$M52, "")</f>
         <v/>
       </c>
-      <c r="M52" s="9" t="str">
-        <f>IF($D52="", (G52/G$75)/($E52/$E$75), "")</f>
+      <c r="U52" s="9" t="str">
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>186</v>
       </c>
@@ -3376,32 +4524,56 @@
         <v>138011</v>
       </c>
       <c r="F53">
-        <f t="shared" ref="F53:G53" si="2">SUMIFS(F$2:F$48,$A$2:$A$48,$A53)-F54</f>
+        <f t="shared" ref="F53:G53" si="19">SUMIFS(F$2:F$48,$A$2:$A$48,$A53)-F54</f>
         <v>30352</v>
       </c>
       <c r="G53">
-        <f t="shared" si="2"/>
+        <f t="shared" si="19"/>
         <v>23243</v>
       </c>
       <c r="I53" s="9">
-        <f>(F53/F$74)/($E53/$E$74)</f>
+        <f t="shared" si="6"/>
+        <v>28.465677872587055</v>
+      </c>
+      <c r="J53" s="9">
+        <f t="shared" si="11"/>
+        <v>17.027483408413882</v>
+      </c>
+      <c r="K53" s="9">
+        <f t="shared" si="12"/>
+        <v>23.643761761863587</v>
+      </c>
+      <c r="M53" s="9">
+        <f t="shared" si="13"/>
+        <v>36.084703396921014</v>
+      </c>
+      <c r="N53" s="9">
+        <f t="shared" si="13"/>
+        <v>23.335844878753864</v>
+      </c>
+      <c r="O53" s="9">
+        <f t="shared" si="13"/>
+        <v>35.858866364281525</v>
+      </c>
+      <c r="Q53" s="9">
+        <f t="shared" si="17"/>
         <v>0.59817593259606328</v>
       </c>
-      <c r="J53" s="9">
-        <f>(G53/G$74)/($E53/$E$74)</f>
+      <c r="R53" s="9">
+        <f t="shared" si="14"/>
         <v>0.83060596229935357</v>
       </c>
-      <c r="K53" s="9"/>
-      <c r="L53" s="9">
-        <f>IF($D53="", (F53/F$75)/($E53/$E$75), "")</f>
-        <v>0.6466963195475518</v>
-      </c>
-      <c r="M53" s="9">
-        <f>IF($D53="", (G53/G$75)/($E53/$E$75), "")</f>
-        <v>0.99374147460336992</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S53" s="9"/>
+      <c r="T53" s="9">
+        <f t="shared" si="18"/>
+        <v>0.64669631954755191</v>
+      </c>
+      <c r="U53" s="9">
+        <f t="shared" si="15"/>
+        <v>0.99374147460337003</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
         <v>242</v>
       </c>
@@ -3410,32 +4582,44 @@
         <v>52235</v>
       </c>
       <c r="F54">
-        <f t="shared" ref="F54:G54" si="3">SUMIFS(F$2:F$48,$A$2:$A$48,$A53,$D$2:$D$48,"Verkehr")</f>
+        <f t="shared" ref="F54:G54" si="20">SUMIFS(F$2:F$48,$A$2:$A$48,$A53,$D$2:$D$48,"Verkehr")</f>
         <v>10863</v>
       </c>
       <c r="G54">
-        <f t="shared" si="3"/>
+        <f t="shared" si="20"/>
         <v>13654</v>
       </c>
       <c r="I54" s="9">
-        <f>(F54/F$74)/($E54/$E$74)</f>
-        <v>0.56564441710160251</v>
+        <f t="shared" si="6"/>
+        <v>10.773812838647535</v>
       </c>
       <c r="J54" s="9">
-        <f>(G54/G$74)/($E54/$E$74)</f>
+        <f t="shared" si="11"/>
+        <v>6.0941470830785454</v>
+      </c>
+      <c r="K54" s="9">
+        <f t="shared" si="12"/>
+        <v>13.889425766746351</v>
+      </c>
+      <c r="Q54" s="9">
+        <f t="shared" si="17"/>
+        <v>0.5656444171016024</v>
+      </c>
+      <c r="R54" s="9">
+        <f t="shared" si="14"/>
         <v>1.2891838734122587</v>
       </c>
-      <c r="K54" s="9"/>
-      <c r="L54" s="9" t="str">
-        <f>IF($D54="", (F54/F$75)/($E54/$E$75), "")</f>
+      <c r="S54" s="9"/>
+      <c r="T54" s="9" t="str">
+        <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="M54" s="9" t="str">
-        <f>IF($D54="", (G54/G$75)/($E54/$E$75), "")</f>
+      <c r="U54" s="9" t="str">
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>187</v>
       </c>
@@ -3447,32 +4631,56 @@
         <v>56724</v>
       </c>
       <c r="F55">
-        <f t="shared" ref="F55:G55" si="4">SUMIFS(F$2:F$48,$A$2:$A$48,$A55)-F56</f>
+        <f t="shared" ref="F55:G55" si="21">SUMIFS(F$2:F$48,$A$2:$A$48,$A55)-F56</f>
         <v>7610</v>
       </c>
       <c r="G55">
-        <f t="shared" si="4"/>
+        <f t="shared" si="21"/>
         <v>4581</v>
       </c>
       <c r="I55" s="9">
-        <f>(F55/F$74)/($E55/$E$74)</f>
-        <v>0.36489938627971169</v>
+        <f t="shared" si="6"/>
+        <v>11.699698659125925</v>
       </c>
       <c r="J55" s="9">
-        <f>(G55/G$74)/($E55/$E$74)</f>
-        <v>0.3982997264819137</v>
-      </c>
-      <c r="K55" s="9"/>
-      <c r="L55" s="9">
-        <f>IF($D55="", (F55/F$75)/($E55/$E$75), "")</f>
-        <v>0.39449780115376548</v>
+        <f t="shared" si="11"/>
+        <v>4.2692128603726163</v>
+      </c>
+      <c r="K55" s="9">
+        <f t="shared" si="12"/>
+        <v>4.659986775850669</v>
       </c>
       <c r="M55" s="9">
-        <f>IF($D55="", (G55/G$75)/($E55/$E$75), "")</f>
+        <f t="shared" si="13"/>
+        <v>14.831199799196787</v>
+      </c>
+      <c r="N55" s="9">
+        <f t="shared" si="13"/>
+        <v>5.850875709255301</v>
+      </c>
+      <c r="O55" s="9">
+        <f t="shared" si="13"/>
+        <v>7.0674812552068866</v>
+      </c>
+      <c r="Q55" s="9">
+        <f t="shared" si="17"/>
+        <v>0.36489938627971175</v>
+      </c>
+      <c r="R55" s="9">
+        <f t="shared" si="14"/>
+        <v>0.39829972648191375</v>
+      </c>
+      <c r="S55" s="9"/>
+      <c r="T55" s="9">
+        <f t="shared" si="18"/>
+        <v>0.39449780115376554</v>
+      </c>
+      <c r="U55" s="9">
+        <f t="shared" si="15"/>
         <v>0.47652795127132197</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
         <v>242</v>
       </c>
@@ -3481,32 +4689,44 @@
         <v>1806</v>
       </c>
       <c r="F56">
-        <f t="shared" ref="F56:G56" si="5">SUMIFS(F$2:F$48,$A$2:$A$48,$A55,$D$2:$D$48,"Verkehr")</f>
+        <f t="shared" ref="F56:G56" si="22">SUMIFS(F$2:F$48,$A$2:$A$48,$A55,$D$2:$D$48,"Verkehr")</f>
         <v>649</v>
       </c>
       <c r="G56">
-        <f t="shared" si="5"/>
+        <f t="shared" si="22"/>
         <v>327</v>
       </c>
       <c r="I56" s="9">
-        <f>(F56/F$74)/($E56/$E$74)</f>
+        <f t="shared" si="6"/>
+        <v>0.37249939669948207</v>
+      </c>
+      <c r="J56" s="9">
+        <f t="shared" si="11"/>
+        <v>0.36408924393979342</v>
+      </c>
+      <c r="K56" s="9">
+        <f t="shared" si="12"/>
+        <v>0.33263821779156705</v>
+      </c>
+      <c r="Q56" s="9">
+        <f t="shared" si="17"/>
         <v>0.97742237213212557</v>
       </c>
-      <c r="J56" s="9">
-        <f>(G56/G$74)/($E56/$E$74)</f>
-        <v>0.89298995042380303</v>
-      </c>
-      <c r="K56" s="9"/>
-      <c r="L56" s="9" t="str">
-        <f>IF($D56="", (F56/F$75)/($E56/$E$75), "")</f>
+      <c r="R56" s="9">
+        <f t="shared" si="14"/>
+        <v>0.89298995042380314</v>
+      </c>
+      <c r="S56" s="9"/>
+      <c r="T56" s="9" t="str">
+        <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="M56" s="9" t="str">
-        <f>IF($D56="", (G56/G$75)/($E56/$E$75), "")</f>
+      <c r="U56" s="9" t="str">
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>188</v>
       </c>
@@ -3518,32 +4738,56 @@
         <v>36717</v>
       </c>
       <c r="F57">
-        <f t="shared" ref="F57:G57" si="6">SUMIFS(F$2:F$48,$A$2:$A$48,$A57)-F58</f>
+        <f t="shared" ref="F57:G57" si="23">SUMIFS(F$2:F$48,$A$2:$A$48,$A57)-F58</f>
         <v>10783</v>
       </c>
       <c r="G57">
+        <f t="shared" si="23"/>
+        <v>5601</v>
+      </c>
+      <c r="I57" s="9">
         <f t="shared" si="6"/>
-        <v>5601</v>
-      </c>
-      <c r="I57" s="9">
-        <f>(F57/F$74)/($E57/$E$74)</f>
-        <v>0.79878102598564049</v>
+        <v>7.573123116619537</v>
       </c>
       <c r="J57" s="9">
-        <f>(G57/G$74)/($E57/$E$74)</f>
-        <v>0.75234137745830298</v>
-      </c>
-      <c r="K57" s="9"/>
-      <c r="L57" s="9">
-        <f>IF($D57="", (F57/F$75)/($E57/$E$75), "")</f>
-        <v>0.8635732758211121</v>
+        <f t="shared" si="11"/>
+        <v>6.0492670530089256</v>
+      </c>
+      <c r="K57" s="9">
+        <f t="shared" si="12"/>
+        <v>5.6975738772188596</v>
       </c>
       <c r="M57" s="9">
-        <f>IF($D57="", (G57/G$75)/($E57/$E$75), "")</f>
-        <v>0.90010530115975129</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="13"/>
+        <v>9.6001192269076299</v>
+      </c>
+      <c r="N57" s="9">
+        <f t="shared" si="13"/>
+        <v>8.2904064090538654</v>
+      </c>
+      <c r="O57" s="9">
+        <f t="shared" si="13"/>
+        <v>8.6411182079052118</v>
+      </c>
+      <c r="Q57" s="9">
+        <f t="shared" si="17"/>
+        <v>0.7987810259856406</v>
+      </c>
+      <c r="R57" s="9">
+        <f t="shared" si="14"/>
+        <v>0.7523413774583031</v>
+      </c>
+      <c r="S57" s="9"/>
+      <c r="T57" s="9">
+        <f t="shared" si="18"/>
+        <v>0.86357327582111221</v>
+      </c>
+      <c r="U57" s="9">
+        <f t="shared" si="15"/>
+        <v>0.9001053011597514</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D58" t="s">
         <v>242</v>
       </c>
@@ -3552,32 +4796,44 @@
         <v>1462</v>
       </c>
       <c r="F58">
-        <f t="shared" ref="F58:G58" si="7">SUMIFS(F$2:F$48,$A$2:$A$48,$A57,$D$2:$D$48,"Verkehr")</f>
+        <f t="shared" ref="F58:G58" si="24">SUMIFS(F$2:F$48,$A$2:$A$48,$A57,$D$2:$D$48,"Verkehr")</f>
         <v>563</v>
       </c>
       <c r="G58">
-        <f t="shared" si="7"/>
+        <f t="shared" si="24"/>
         <v>367</v>
       </c>
       <c r="I58" s="9">
-        <f>(F58/F$74)/($E58/$E$74)</f>
+        <f t="shared" si="6"/>
+        <v>0.30154713066148547</v>
+      </c>
+      <c r="J58" s="9">
+        <f t="shared" si="11"/>
+        <v>0.31584321161495177</v>
+      </c>
+      <c r="K58" s="9">
+        <f t="shared" si="12"/>
+        <v>0.37332790804130006</v>
+      </c>
+      <c r="Q58" s="9">
+        <f t="shared" si="17"/>
         <v>1.047409109554801</v>
       </c>
-      <c r="J58" s="9">
-        <f>(G58/G$74)/($E58/$E$74)</f>
-        <v>1.238041652800189</v>
-      </c>
-      <c r="K58" s="9"/>
-      <c r="L58" s="9" t="str">
-        <f>IF($D58="", (F58/F$75)/($E58/$E$75), "")</f>
+      <c r="R58" s="9">
+        <f t="shared" si="14"/>
+        <v>1.2380416528001892</v>
+      </c>
+      <c r="S58" s="9"/>
+      <c r="T58" s="9" t="str">
+        <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="M58" s="9" t="str">
-        <f>IF($D58="", (G58/G$75)/($E58/$E$75), "")</f>
+      <c r="U58" s="9" t="str">
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>189</v>
       </c>
@@ -3589,32 +4845,56 @@
         <v>11807</v>
       </c>
       <c r="F59">
-        <f t="shared" ref="F59:G59" si="8">SUMIFS(F$2:F$48,$A$2:$A$48,$A59)-F60</f>
+        <f t="shared" ref="F59:G59" si="25">SUMIFS(F$2:F$48,$A$2:$A$48,$A59)-F60</f>
         <v>3613</v>
       </c>
       <c r="G59">
-        <f t="shared" si="8"/>
+        <f t="shared" si="25"/>
         <v>856</v>
       </c>
       <c r="I59" s="9">
-        <f>(F59/F$74)/($E59/$E$74)</f>
-        <v>0.83230733656435363</v>
+        <f t="shared" si="6"/>
+        <v>2.4352715264843772</v>
       </c>
       <c r="J59" s="9">
-        <f>(G59/G$74)/($E59/$E$74)</f>
+        <f t="shared" si="11"/>
+        <v>2.02689435801922</v>
+      </c>
+      <c r="K59" s="9">
+        <f t="shared" si="12"/>
+        <v>0.8707593713442856</v>
+      </c>
+      <c r="M59" s="9">
+        <f t="shared" si="13"/>
+        <v>3.0870879350736278</v>
+      </c>
+      <c r="N59" s="9">
+        <f t="shared" si="13"/>
+        <v>2.77782049113527</v>
+      </c>
+      <c r="O59" s="9">
+        <f t="shared" si="13"/>
+        <v>1.3206208152056527</v>
+      </c>
+      <c r="Q59" s="9">
+        <f t="shared" si="17"/>
+        <v>0.83230733656435374</v>
+      </c>
+      <c r="R59" s="9">
+        <f t="shared" si="14"/>
         <v>0.35756151290502586</v>
       </c>
-      <c r="K59" s="9"/>
-      <c r="L59" s="9">
-        <f>IF($D59="", (F59/F$75)/($E59/$E$75), "")</f>
+      <c r="S59" s="9"/>
+      <c r="T59" s="9">
+        <f t="shared" si="18"/>
         <v>0.89981903643733374</v>
       </c>
-      <c r="M59" s="9">
-        <f>IF($D59="", (G59/G$75)/($E59/$E$75), "")</f>
+      <c r="U59" s="9">
+        <f t="shared" si="15"/>
         <v>0.42778853177506121</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
         <v>242</v>
       </c>
@@ -3623,32 +4903,44 @@
         <v>165</v>
       </c>
       <c r="F60">
-        <f t="shared" ref="F60:G60" si="9">SUMIFS(F$2:F$48,$A$2:$A$48,$A59,$D$2:$D$48,"Verkehr")</f>
+        <f t="shared" ref="F60:G60" si="26">SUMIFS(F$2:F$48,$A$2:$A$48,$A59,$D$2:$D$48,"Verkehr")</f>
         <v>221</v>
       </c>
       <c r="G60">
-        <f t="shared" si="9"/>
+        <f t="shared" si="26"/>
         <v>11</v>
       </c>
       <c r="I60" s="9">
-        <f>(F60/F$74)/($E60/$E$74)</f>
-        <v>3.6430376028351938</v>
+        <f t="shared" si="6"/>
+        <v>3.4032336907759989E-2</v>
       </c>
       <c r="J60" s="9">
-        <f>(G60/G$74)/($E60/$E$74)</f>
+        <f t="shared" si="11"/>
+        <v>0.12398108306732565</v>
+      </c>
+      <c r="K60" s="9">
+        <f t="shared" si="12"/>
+        <v>1.1189664818676568E-2</v>
+      </c>
+      <c r="Q60" s="9">
+        <f t="shared" si="17"/>
+        <v>3.6430376028351943</v>
+      </c>
+      <c r="R60" s="9">
+        <f t="shared" si="14"/>
         <v>0.3287950765474798</v>
       </c>
-      <c r="K60" s="9"/>
-      <c r="L60" s="9" t="str">
-        <f>IF($D60="", (F60/F$75)/($E60/$E$75), "")</f>
+      <c r="S60" s="9"/>
+      <c r="T60" s="9" t="str">
+        <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="M60" s="9" t="str">
-        <f>IF($D60="", (G60/G$75)/($E60/$E$75), "")</f>
+      <c r="U60" s="9" t="str">
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>190</v>
       </c>
@@ -3660,32 +4952,56 @@
         <v>79541</v>
       </c>
       <c r="F61">
-        <f t="shared" ref="F61:G61" si="10">SUMIFS(F$2:F$48,$A$2:$A$48,$A61)-F62</f>
+        <f t="shared" ref="F61:G61" si="27">SUMIFS(F$2:F$48,$A$2:$A$48,$A61)-F62</f>
         <v>34046</v>
       </c>
       <c r="G61">
-        <f t="shared" si="10"/>
+        <f t="shared" si="27"/>
         <v>9266</v>
       </c>
       <c r="I61" s="9">
-        <f>(F61/F$74)/($E61/$E$74)</f>
+        <f t="shared" si="6"/>
+        <v>16.405855212000834</v>
+      </c>
+      <c r="J61" s="9">
+        <f t="shared" si="11"/>
+        <v>19.099818796878594</v>
+      </c>
+      <c r="K61" s="9">
+        <f t="shared" si="12"/>
+        <v>9.4257667463506429</v>
+      </c>
+      <c r="M61" s="9">
+        <f t="shared" si="13"/>
+        <v>20.796990043507364</v>
+      </c>
+      <c r="N61" s="9">
+        <f t="shared" si="13"/>
+        <v>26.175941445112482</v>
+      </c>
+      <c r="O61" s="9">
+        <f t="shared" si="13"/>
+        <v>14.295411768335956</v>
+      </c>
+      <c r="Q61" s="9">
+        <f t="shared" si="17"/>
         <v>1.1642074460651788</v>
       </c>
-      <c r="J61" s="9">
-        <f>(G61/G$74)/($E61/$E$74)</f>
+      <c r="R61" s="9">
+        <f t="shared" si="14"/>
         <v>0.57453675072395638</v>
       </c>
-      <c r="K61" s="9"/>
-      <c r="L61" s="9">
-        <f>IF($D61="", (F61/F$75)/($E61/$E$75), "")</f>
+      <c r="S61" s="9"/>
+      <c r="T61" s="9">
+        <f t="shared" si="18"/>
         <v>1.2586408605453163</v>
       </c>
-      <c r="M61" s="9">
-        <f>IF($D61="", (G61/G$75)/($E61/$E$75), "")</f>
+      <c r="U61" s="9">
+        <f t="shared" si="15"/>
         <v>0.68737888215698106</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
         <v>242</v>
       </c>
@@ -3694,32 +5010,44 @@
         <v>9247</v>
       </c>
       <c r="F62">
-        <f t="shared" ref="F62:G62" si="11">SUMIFS(F$2:F$48,$A$2:$A$48,$A61,$D$2:$D$48,"Verkehr")</f>
+        <f t="shared" ref="F62:G62" si="28">SUMIFS(F$2:F$48,$A$2:$A$48,$A61,$D$2:$D$48,"Verkehr")</f>
         <v>3494</v>
       </c>
       <c r="G62">
+        <f t="shared" si="28"/>
+        <v>1959</v>
+      </c>
+      <c r="I62" s="9">
+        <f t="shared" si="6"/>
+        <v>1.9072546629457978</v>
+      </c>
+      <c r="J62" s="9">
         <f t="shared" si="11"/>
-        <v>1959</v>
-      </c>
-      <c r="I62" s="9">
-        <f>(F62/F$74)/($E62/$E$74)</f>
+        <v>1.9601353132906598</v>
+      </c>
+      <c r="K62" s="9">
+        <f t="shared" si="12"/>
+        <v>1.9927775799806724</v>
+      </c>
+      <c r="Q62" s="9">
+        <f t="shared" si="17"/>
         <v>1.0277260563952098</v>
       </c>
-      <c r="J62" s="9">
-        <f>(G62/G$74)/($E62/$E$74)</f>
+      <c r="R62" s="9">
+        <f t="shared" si="14"/>
         <v>1.044840848312717</v>
       </c>
-      <c r="K62" s="9"/>
-      <c r="L62" s="9" t="str">
-        <f>IF($D62="", (F62/F$75)/($E62/$E$75), "")</f>
+      <c r="S62" s="9"/>
+      <c r="T62" s="9" t="str">
+        <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="M62" s="9" t="str">
-        <f>IF($D62="", (G62/G$75)/($E62/$E$75), "")</f>
+      <c r="U62" s="9" t="str">
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>191</v>
       </c>
@@ -3731,32 +5059,56 @@
         <v>2733</v>
       </c>
       <c r="F63">
-        <f t="shared" ref="F63:G63" si="12">SUMIFS(F$2:F$48,$A$2:$A$48,$A63)-F64</f>
+        <f t="shared" ref="F63:G63" si="29">SUMIFS(F$2:F$48,$A$2:$A$48,$A63)-F64</f>
         <v>1259</v>
       </c>
       <c r="G63">
+        <f t="shared" si="29"/>
+        <v>779</v>
+      </c>
+      <c r="I63" s="9">
+        <f t="shared" si="6"/>
+        <v>0.56369925314489733</v>
+      </c>
+      <c r="J63" s="9">
+        <f t="shared" si="11"/>
+        <v>0.70629947322064701</v>
+      </c>
+      <c r="K63" s="9">
         <f t="shared" si="12"/>
-        <v>779</v>
-      </c>
-      <c r="I63" s="9">
-        <f>(F63/F$74)/($E63/$E$74)</f>
+        <v>0.79243171761354969</v>
+      </c>
+      <c r="M63" s="9">
+        <f t="shared" si="13"/>
+        <v>0.71457705823293172</v>
+      </c>
+      <c r="N63" s="9">
+        <f t="shared" si="13"/>
+        <v>0.96797010748389278</v>
+      </c>
+      <c r="O63" s="9">
+        <f t="shared" si="13"/>
+        <v>1.2018266530901911</v>
+      </c>
+      <c r="Q63" s="9">
+        <f t="shared" si="17"/>
         <v>1.2529721642882765</v>
       </c>
-      <c r="J63" s="9">
-        <f>(G63/G$74)/($E63/$E$74)</f>
-        <v>1.4057703876536047</v>
-      </c>
-      <c r="K63" s="9"/>
-      <c r="L63" s="9">
-        <f>IF($D63="", (F63/F$75)/($E63/$E$75), "")</f>
-        <v>1.354605631865055</v>
-      </c>
-      <c r="M63" s="9">
-        <f>IF($D63="", (G63/G$75)/($E63/$E$75), "")</f>
-        <v>1.6818713100895968</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="R63" s="9">
+        <f t="shared" si="14"/>
+        <v>1.4057703876536045</v>
+      </c>
+      <c r="S63" s="9"/>
+      <c r="T63" s="9">
+        <f t="shared" si="18"/>
+        <v>1.3546056318650552</v>
+      </c>
+      <c r="U63" s="9">
+        <f t="shared" si="15"/>
+        <v>1.681871310089597</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
         <v>242</v>
       </c>
@@ -3765,32 +5117,44 @@
         <v>617</v>
       </c>
       <c r="F64">
-        <f t="shared" ref="F64:G64" si="13">SUMIFS(F$2:F$48,$A$2:$A$48,$A63,$D$2:$D$48,"Verkehr")</f>
+        <f t="shared" ref="F64:G64" si="30">SUMIFS(F$2:F$48,$A$2:$A$48,$A63,$D$2:$D$48,"Verkehr")</f>
         <v>396</v>
       </c>
       <c r="G64">
-        <f t="shared" si="13"/>
+        <f t="shared" si="30"/>
         <v>302</v>
       </c>
       <c r="I64" s="9">
-        <f>(F64/F$74)/($E64/$E$74)</f>
+        <f t="shared" si="6"/>
+        <v>0.1272603143762904</v>
+      </c>
+      <c r="J64" s="9">
+        <f t="shared" si="11"/>
+        <v>0.22215614884461973</v>
+      </c>
+      <c r="K64" s="9">
+        <f t="shared" si="12"/>
+        <v>0.30720716138548393</v>
+      </c>
+      <c r="Q64" s="9">
+        <f t="shared" si="17"/>
         <v>1.7456828543400893</v>
       </c>
-      <c r="J64" s="9">
-        <f>(G64/G$74)/($E64/$E$74)</f>
-        <v>2.4140059915074286</v>
-      </c>
-      <c r="K64" s="9"/>
-      <c r="L64" s="9" t="str">
-        <f>IF($D64="", (F64/F$75)/($E64/$E$75), "")</f>
+      <c r="R64" s="9">
+        <f t="shared" si="14"/>
+        <v>2.4140059915074281</v>
+      </c>
+      <c r="S64" s="9"/>
+      <c r="T64" s="9" t="str">
+        <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="M64" s="9" t="str">
-        <f>IF($D64="", (G64/G$75)/($E64/$E$75), "")</f>
+      <c r="U64" s="9" t="str">
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>192</v>
       </c>
@@ -3802,32 +5166,56 @@
         <v>30615</v>
       </c>
       <c r="F65">
-        <f t="shared" ref="F65:G65" si="14">SUMIFS(F$2:F$48,$A$2:$A$48,$A65)-F66</f>
+        <f t="shared" ref="F65:G65" si="31">SUMIFS(F$2:F$48,$A$2:$A$48,$A65)-F66</f>
         <v>5266</v>
       </c>
       <c r="G65">
+        <f t="shared" si="31"/>
+        <v>1883</v>
+      </c>
+      <c r="I65" s="9">
+        <f t="shared" si="6"/>
+        <v>6.314545420794377</v>
+      </c>
+      <c r="J65" s="9">
+        <f t="shared" si="11"/>
+        <v>2.9542279793327459</v>
+      </c>
+      <c r="K65" s="9">
+        <f t="shared" si="12"/>
+        <v>1.9154671685061797</v>
+      </c>
+      <c r="M65" s="9">
+        <f t="shared" si="13"/>
+        <v>8.0046749497991971</v>
+      </c>
+      <c r="N65" s="9">
+        <f t="shared" si="13"/>
+        <v>4.0487137299524854</v>
+      </c>
+      <c r="O65" s="9">
+        <f t="shared" si="13"/>
+        <v>2.9050572371872012</v>
+      </c>
+      <c r="Q65" s="9">
+        <f t="shared" si="17"/>
+        <v>0.46784491716604054</v>
+      </c>
+      <c r="R65" s="9">
         <f t="shared" si="14"/>
-        <v>1883</v>
-      </c>
-      <c r="I65" s="9">
-        <f>(F65/F$74)/($E65/$E$74)</f>
-        <v>0.4678449171660406</v>
-      </c>
-      <c r="J65" s="9">
-        <f>(G65/G$74)/($E65/$E$74)</f>
-        <v>0.30334205249333879</v>
-      </c>
-      <c r="K65" s="9"/>
-      <c r="L65" s="9">
-        <f>IF($D65="", (F65/F$75)/($E65/$E$75), "")</f>
-        <v>0.50579364625593581</v>
-      </c>
-      <c r="M65" s="9">
-        <f>IF($D65="", (G65/G$75)/($E65/$E$75), "")</f>
+        <v>0.30334205249333873</v>
+      </c>
+      <c r="S65" s="9"/>
+      <c r="T65" s="9">
+        <f t="shared" si="18"/>
+        <v>0.5057936462559357</v>
+      </c>
+      <c r="U65" s="9">
+        <f t="shared" si="15"/>
         <v>0.36292007550663585</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
         <v>242</v>
       </c>
@@ -3836,32 +5224,44 @@
         <v>22564</v>
       </c>
       <c r="F66">
-        <f t="shared" ref="F66:G66" si="15">SUMIFS(F$2:F$48,$A$2:$A$48,$A65,$D$2:$D$48,"Verkehr")</f>
+        <f t="shared" ref="F66:G66" si="32">SUMIFS(F$2:F$48,$A$2:$A$48,$A65,$D$2:$D$48,"Verkehr")</f>
         <v>1561</v>
       </c>
       <c r="G66">
+        <f t="shared" si="32"/>
+        <v>683</v>
+      </c>
+      <c r="I66" s="9">
+        <f t="shared" si="6"/>
+        <v>4.6539736362830091</v>
+      </c>
+      <c r="J66" s="9">
+        <f t="shared" si="11"/>
+        <v>0.87572158673346312</v>
+      </c>
+      <c r="K66" s="9">
+        <f t="shared" si="12"/>
+        <v>0.69477646101419055</v>
+      </c>
+      <c r="Q66" s="9">
+        <f t="shared" si="17"/>
+        <v>0.18816642619249471</v>
+      </c>
+      <c r="R66" s="9">
+        <f t="shared" si="14"/>
+        <v>0.14928672040546578</v>
+      </c>
+      <c r="S66" s="9"/>
+      <c r="T66" s="9" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="U66" s="9" t="str">
         <f t="shared" si="15"/>
-        <v>683</v>
-      </c>
-      <c r="I66" s="9">
-        <f>(F66/F$74)/($E66/$E$74)</f>
-        <v>0.18816642619249474</v>
-      </c>
-      <c r="J66" s="9">
-        <f>(G66/G$74)/($E66/$E$74)</f>
-        <v>0.14928672040546578</v>
-      </c>
-      <c r="K66" s="9"/>
-      <c r="L66" s="9" t="str">
-        <f>IF($D66="", (F66/F$75)/($E66/$E$75), "")</f>
         <v/>
       </c>
-      <c r="M66" s="9" t="str">
-        <f>IF($D66="", (G66/G$75)/($E66/$E$75), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>246</v>
       </c>
@@ -3870,32 +5270,56 @@
         <v>7532</v>
       </c>
       <c r="F67">
-        <f t="shared" ref="F67:G67" si="16">SUMIFS(F$2:F$48,$A$2:$A$48,$A67)-F68</f>
+        <f t="shared" ref="F67:G67" si="33">SUMIFS(F$2:F$48,$A$2:$A$48,$A67)-F68</f>
         <v>17297</v>
       </c>
       <c r="G67">
-        <f t="shared" si="16"/>
+        <f t="shared" si="33"/>
         <v>8513</v>
       </c>
       <c r="I67" s="9">
-        <f>(F67/F$74)/($E67/$E$74)</f>
-        <v>6.2461987427877297</v>
+        <f t="shared" ref="I67:I69" si="34">100*E67/E$74</f>
+        <v>1.5535246156924136</v>
       </c>
       <c r="J67" s="9">
-        <f>(G67/G$74)/($E67/$E$74)</f>
+        <f t="shared" si="11"/>
+        <v>9.7036235014277459</v>
+      </c>
+      <c r="K67" s="9">
+        <f t="shared" si="12"/>
+        <v>8.6597833273994205</v>
+      </c>
+      <c r="M67" s="9">
+        <f t="shared" si="13"/>
+        <v>1.9693356760374832</v>
+      </c>
+      <c r="N67" s="9">
+        <f t="shared" si="13"/>
+        <v>13.298633001706825</v>
+      </c>
+      <c r="O67" s="9">
+        <f t="shared" si="13"/>
+        <v>13.133697429726311</v>
+      </c>
+      <c r="Q67" s="9">
+        <f t="shared" si="17"/>
+        <v>6.2461987427877306</v>
+      </c>
+      <c r="R67" s="9">
+        <f t="shared" si="14"/>
         <v>5.574281372773557</v>
       </c>
-      <c r="K67" s="9"/>
-      <c r="L67" s="9">
-        <f>IF($D67="", (F67/F$75)/($E67/$E$75), "")</f>
+      <c r="S67" s="9"/>
+      <c r="T67" s="9">
+        <f t="shared" si="18"/>
         <v>6.7528523265597444</v>
       </c>
-      <c r="M67" s="9">
-        <f>IF($D67="", (G67/G$75)/($E67/$E$75), "")</f>
+      <c r="U67" s="9">
+        <f t="shared" si="15"/>
         <v>6.6691004431264522</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D68" t="s">
         <v>242</v>
       </c>
@@ -3904,32 +5328,44 @@
         <v>7975</v>
       </c>
       <c r="F68">
-        <f t="shared" ref="F68:G68" si="17">SUMIFS(F$2:F$48,$A$2:$A$48,$A67,$D$2:$D$48,"Verkehr")</f>
+        <f t="shared" ref="F68:G68" si="35">SUMIFS(F$2:F$48,$A$2:$A$48,$A67,$D$2:$D$48,"Verkehr")</f>
         <v>5536</v>
       </c>
       <c r="G68">
+        <f t="shared" si="35"/>
+        <v>5056</v>
+      </c>
+      <c r="I68" s="9">
+        <f t="shared" si="34"/>
+        <v>1.6448962838750663</v>
+      </c>
+      <c r="J68" s="9">
+        <f t="shared" si="11"/>
+        <v>3.1056980808177141</v>
+      </c>
+      <c r="K68" s="9">
+        <f t="shared" si="12"/>
+        <v>5.1431768475662478</v>
+      </c>
+      <c r="Q68" s="9">
         <f t="shared" si="17"/>
-        <v>5056</v>
-      </c>
-      <c r="I68" s="9">
-        <f>(F68/F$74)/($E68/$E$74)</f>
-        <v>1.8880814014007457</v>
-      </c>
-      <c r="J68" s="9">
-        <f>(G68/G$74)/($E68/$E$74)</f>
-        <v>3.1267484144653119</v>
-      </c>
-      <c r="K68" s="9"/>
-      <c r="L68" s="9" t="str">
-        <f>IF($D68="", (F68/F$75)/($E68/$E$75), "")</f>
+        <v>1.8880814014007459</v>
+      </c>
+      <c r="R68" s="9">
+        <f t="shared" si="14"/>
+        <v>3.1267484144653124</v>
+      </c>
+      <c r="S68" s="9"/>
+      <c r="T68" s="9" t="str">
+        <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="M68" s="9" t="str">
-        <f>IF($D68="", (G68/G$75)/($E68/$E$75), "")</f>
+      <c r="U68" s="9" t="str">
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>193</v>
       </c>
@@ -3949,29 +5385,42 @@
         <v>10717</v>
       </c>
       <c r="I69" s="9">
-        <f>(F69/F$74)/($E69/$E$74)</f>
+        <f t="shared" si="34"/>
+        <v>1.0547961875532399</v>
+      </c>
+      <c r="J69" s="9">
+        <f t="shared" si="11"/>
+        <v>13.615479122371012</v>
+      </c>
+      <c r="K69" s="9">
+        <f t="shared" si="12"/>
+        <v>10.901785260159707</v>
+      </c>
+      <c r="M69" s="9"/>
+      <c r="Q69" s="9">
+        <f t="shared" si="17"/>
         <v>12.908161105468333</v>
       </c>
-      <c r="J69" s="9">
-        <f>(G69/G$74)/($E69/$E$74)</f>
+      <c r="R69" s="9">
+        <f t="shared" si="14"/>
         <v>10.335442418926499</v>
       </c>
-      <c r="K69" s="9"/>
-      <c r="L69" s="9" t="str">
-        <f>IF($D69="", (F69/F$75)/($E69/$E$75), "")</f>
+      <c r="S69" s="9"/>
+      <c r="T69" s="9" t="str">
+        <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="M69" s="9" t="str">
-        <f>IF($D69="", (G69/G$75)/($E69/$E$75), "")</f>
+      <c r="U69" s="9" t="str">
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>247</v>
       </c>
@@ -3987,12 +5436,12 @@
         <f>G74-G73</f>
         <v>75535</v>
       </c>
-      <c r="I72" s="9"/>
-      <c r="J72" s="9"/>
-      <c r="L72" s="9"/>
-      <c r="M72" s="9"/>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q72" s="9"/>
+      <c r="R72" s="9"/>
+      <c r="T72" s="9"/>
+      <c r="U72" s="9"/>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>242</v>
       </c>
@@ -4008,12 +5457,12 @@
         <f>SUMIFS(G$2:G$48,$D$2:$D$48,"Verkehr")</f>
         <v>22770</v>
       </c>
-      <c r="I73" s="9"/>
-      <c r="J73" s="9"/>
-      <c r="L73" s="9"/>
-      <c r="M73" s="9"/>
-    </row>
-    <row r="74" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q73" s="9"/>
+      <c r="R73" s="9"/>
+      <c r="T73" s="9"/>
+      <c r="U73" s="9"/>
+    </row>
+    <row r="74" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="12" t="s">
         <v>250</v>
       </c>
@@ -4029,12 +5478,12 @@
         <f>SUM(G$2:G$48)</f>
         <v>98305</v>
       </c>
-      <c r="I74" s="13"/>
-      <c r="J74" s="13"/>
-      <c r="L74" s="13"/>
-      <c r="M74" s="13"/>
-    </row>
-    <row r="75" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q74" s="13"/>
+      <c r="R74" s="13"/>
+      <c r="T74" s="13"/>
+      <c r="U74" s="13"/>
+    </row>
+    <row r="75" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
         <v>248</v>
       </c>
@@ -4050,12 +5499,12 @@
         <f>G72-G48</f>
         <v>64818</v>
       </c>
-      <c r="I75" s="16"/>
-      <c r="J75" s="16"/>
-      <c r="L75" s="16"/>
-      <c r="M75" s="16"/>
-    </row>
-    <row r="77" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q75" s="16"/>
+      <c r="R75" s="16"/>
+      <c r="T75" s="16"/>
+      <c r="U75" s="16"/>
+    </row>
+    <row r="77" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
         <v>245</v>
       </c>
@@ -4073,23 +5522,23 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I2:J49 I72:J75 L2:M49 L72:M75">
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="Q72:R75 T72:U75 Q2:R49 T2:U49">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I51:K69">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="Q51:S69">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L51:M69">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="T51:U69">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L51:M69">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="T51:U69">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4100,7 +5549,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7424,7 +8873,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7447,23 +8896,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="849ba905-b147-4d5f-9c8c-24526156989e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A8B81505B058D246836E19FAAE35149D" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4d331c3ec03db8e3d45aa8d211ccdb8a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="849ba905-b147-4d5f-9c8c-24526156989e" xmlns:ns4="6e1ea3c6-49aa-46a0-abdd-da3db8966731" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3a8779806608e9e8be67f7791cfedb9b" ns3:_="" ns4:_="">
     <xsd:import namespace="849ba905-b147-4d5f-9c8c-24526156989e"/>
@@ -7702,10 +9134,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="849ba905-b147-4d5f-9c8c-24526156989e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E3F9E17-51B7-4277-BC53-B62A92A491D0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C192A6EB-51FA-4D29-89B9-E9C0800E22DC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="849ba905-b147-4d5f-9c8c-24526156989e"/>
+    <ds:schemaRef ds:uri="6e1ea3c6-49aa-46a0-abdd-da3db8966731"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7728,20 +9188,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C192A6EB-51FA-4D29-89B9-E9C0800E22DC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E3F9E17-51B7-4277-BC53-B62A92A491D0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="849ba905-b147-4d5f-9c8c-24526156989e"/>
-    <ds:schemaRef ds:uri="6e1ea3c6-49aa-46a0-abdd-da3db8966731"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>